<commit_message>
Reorganize by neut. antibody type, Add CC12.3 files and submission
</commit_message>
<xml_diff>
--- a/docking/HADDOCK_Results.xlsx
+++ b/docking/HADDOCK_Results.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colbyford/Documents/SARS-CoV-2_B.1.1.529_Spike-RBD_Predictions/docking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BCB959-32FF-3147-9F4E-0718798CC868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCD4562-CB05-4547-A1B5-EF2100241A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10900" yWindow="460" windowWidth="17960" windowHeight="15840" xr2:uid="{05BB3759-F2AC-475A-81D0-60BB4FF9CDA1}"/>
+    <workbookView xWindow="2960" yWindow="460" windowWidth="25900" windowHeight="15840" xr2:uid="{05BB3759-F2AC-475A-81D0-60BB4FF9CDA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Z$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Y$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,20 +37,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>HLA Active Residues</t>
   </si>
   <si>
-    <t>CSP Active Residues</t>
-  </si>
-  <si>
     <t>9,11,22,24,54,62,65,66,72,73,76,209,211,213,227,228,230,237,256,260,261,264,267,270,274,278,281,282</t>
   </si>
   <si>
-    <t>1,2,3,4,5,6</t>
-  </si>
-  <si>
     <t>Fab Name</t>
   </si>
   <si>
@@ -151,6 +145,42 @@
   </si>
   <si>
     <t>`406,408,420,424,452,456,458,459,480,481,487,489,490,492,496,501,503,504,508</t>
+  </si>
+  <si>
+    <t>C105</t>
+  </si>
+  <si>
+    <t>6xcm</t>
+  </si>
+  <si>
+    <t>CC12.3</t>
+  </si>
+  <si>
+    <t>CV07-250</t>
+  </si>
+  <si>
+    <t>6XKP</t>
+  </si>
+  <si>
+    <t>CV30</t>
+  </si>
+  <si>
+    <t>6XE1</t>
+  </si>
+  <si>
+    <t>6XC7 Chain A</t>
+  </si>
+  <si>
+    <t>6xc7_chainsCD_Fab_renumbered.pdb</t>
+  </si>
+  <si>
+    <t>6xc7_chainA_RBD_renumbered.pdb</t>
+  </si>
+  <si>
+    <t>SRBC_6XC7_CC123</t>
+  </si>
+  <si>
+    <t>SRBC_pred_CC123</t>
   </si>
 </sst>
 </file>
@@ -518,13 +548,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C05FAB-699E-4769-A909-822D635E1B9A}">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:Y8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -535,263 +565,329 @@
     <col min="4" max="4" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="91.1640625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26" customWidth="1"/>
-    <col min="9" max="9" width="28.6640625" customWidth="1"/>
-    <col min="10" max="10" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5" customWidth="1"/>
-    <col min="13" max="17" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
+    <col min="8" max="8" width="28.6640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.5" customWidth="1"/>
+    <col min="12" max="16" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="243" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="243" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
       </c>
       <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="64" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
         <v>1</v>
       </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="U1" s="2" t="s">
+      <c r="G2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3">
+        <v>-198.6</v>
+      </c>
+      <c r="K2" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="L2" s="3">
+        <v>95</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="O2" s="3">
+        <v>-106.9</v>
+      </c>
+      <c r="P2" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>-342.6</v>
+      </c>
+      <c r="R2" s="3">
+        <v>10.1</v>
+      </c>
+      <c r="S2" s="3">
+        <v>-37.5</v>
+      </c>
+      <c r="T2" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="U2" s="3">
+        <v>143.19999999999999</v>
+      </c>
+      <c r="V2" s="3">
+        <v>32</v>
+      </c>
+      <c r="W2" s="3">
+        <v>2778.5</v>
+      </c>
+      <c r="X2" s="3">
+        <v>63.1</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="80" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="V1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>22</v>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="3">
+        <v>-163.30000000000001</v>
+      </c>
+      <c r="K3" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="L3" s="3">
+        <v>51</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="O3" s="3">
+        <v>-90.7</v>
+      </c>
+      <c r="P3" s="3">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>-284.89999999999998</v>
+      </c>
+      <c r="R3" s="3">
+        <v>24.1</v>
+      </c>
+      <c r="S3" s="3">
+        <v>-28.8</v>
+      </c>
+      <c r="T3" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="U3" s="3">
+        <v>152.6</v>
+      </c>
+      <c r="V3" s="3">
+        <v>46.9</v>
+      </c>
+      <c r="W3" s="3">
+        <v>2584.3000000000002</v>
+      </c>
+      <c r="X3" s="3">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>-2.6</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="64" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="4" spans="1:25" ht="64" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="H4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="80" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
         <v>37</v>
-      </c>
-      <c r="J2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2" s="3">
-        <v>-198.6</v>
-      </c>
-      <c r="L2" s="3">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="M2" s="3">
-        <v>95</v>
-      </c>
-      <c r="N2" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="O2" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="P2" s="3">
-        <v>-106.9</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="R2" s="3">
-        <v>-342.6</v>
-      </c>
-      <c r="S2" s="3">
-        <v>10.1</v>
-      </c>
-      <c r="T2" s="3">
-        <v>-37.5</v>
-      </c>
-      <c r="U2" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="V2" s="3">
-        <v>143.19999999999999</v>
-      </c>
-      <c r="W2" s="3">
-        <v>32</v>
-      </c>
-      <c r="X2" s="3">
-        <v>2778.5</v>
-      </c>
-      <c r="Y2" s="3">
-        <v>63.1</v>
-      </c>
-      <c r="Z2" s="3">
-        <v>-2.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="80" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" t="b">
-        <v>1</v>
-      </c>
-      <c r="K3" s="3">
-        <v>-163.30000000000001</v>
-      </c>
-      <c r="L3" s="3">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="M3" s="3">
-        <v>51</v>
-      </c>
-      <c r="N3" s="3">
-        <v>0.7</v>
-      </c>
-      <c r="O3" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="P3" s="3">
-        <v>-90.7</v>
-      </c>
-      <c r="Q3" s="3">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="R3" s="3">
-        <v>-284.89999999999998</v>
-      </c>
-      <c r="S3" s="3">
-        <v>24.1</v>
-      </c>
-      <c r="T3" s="3">
-        <v>-28.8</v>
-      </c>
-      <c r="U3" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="V3" s="3">
-        <v>152.6</v>
-      </c>
-      <c r="W3" s="3">
-        <v>46.9</v>
-      </c>
-      <c r="X3" s="3">
-        <v>2584.3000000000002</v>
-      </c>
-      <c r="Y3" s="3">
-        <v>68.400000000000006</v>
-      </c>
-      <c r="Z3" s="3">
-        <v>-2.6</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z3" xr:uid="{30842AB1-A644-42C7-A90C-F34DF0E50414}"/>
+  <autoFilter ref="A1:Y3" xr:uid="{30842AB1-A644-42C7-A90C-F34DF0E50414}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Add 7T9J actual RBD docking submissions
</commit_message>
<xml_diff>
--- a/docking/HADDOCK_Results.xlsx
+++ b/docking/HADDOCK_Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby\Documents\GitHub\SARS-CoV-2_B.1.1.529_Spike-RBD_Predictions\docking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E56DEB6-1D2A-4E69-B90F-DF529CE19379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B665BA9-D93C-4DD1-9225-B1A38F63729F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{05BB3759-F2AC-475A-81D0-60BB4FF9CDA1}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{05BB3759-F2AC-475A-81D0-60BB4FF9CDA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="101">
   <si>
     <t>Fab PDB</t>
   </si>
@@ -321,6 +321,27 @@
   </si>
   <si>
     <t>RoseTTAFold vs. Reference</t>
+  </si>
+  <si>
+    <t>7T9J Chain C</t>
+  </si>
+  <si>
+    <t>SRBC_7T9J_CC121</t>
+  </si>
+  <si>
+    <t>7t9j_chainC_RBD_renumbered.pdb</t>
+  </si>
+  <si>
+    <t>SRBC_7T9J_CC123</t>
+  </si>
+  <si>
+    <t>SRBC_7T9J_CV30</t>
+  </si>
+  <si>
+    <t>SRBC_7T9J_C105</t>
+  </si>
+  <si>
+    <t>Validation</t>
   </si>
 </sst>
 </file>
@@ -729,13 +750,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C05FAB-699E-4769-A909-822D635E1B9A}">
-  <dimension ref="A1:Z21"/>
+  <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,156 +1253,108 @@
         <v>-1.8</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>38</v>
+    <row r="7" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" t="s">
-        <v>37</v>
+        <v>67</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" t="s">
-        <v>40</v>
+        <v>100</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
-      <c r="J7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <v>-161.5</v>
-      </c>
-      <c r="L7">
-        <v>4.8</v>
-      </c>
-      <c r="M7">
-        <v>55</v>
-      </c>
-      <c r="N7">
-        <v>0.8</v>
-      </c>
-      <c r="O7">
-        <v>0.6</v>
-      </c>
-      <c r="P7">
-        <v>-86.1</v>
-      </c>
-      <c r="Q7">
-        <v>2.9</v>
-      </c>
-      <c r="R7">
-        <v>-248.1</v>
-      </c>
-      <c r="S7">
-        <v>24.3</v>
-      </c>
-      <c r="T7">
-        <v>-41.7</v>
-      </c>
-      <c r="U7">
-        <v>2.8</v>
-      </c>
-      <c r="V7">
-        <v>159.1</v>
-      </c>
-      <c r="W7">
-        <v>14.7</v>
-      </c>
-      <c r="X7">
-        <v>2489.8000000000002</v>
-      </c>
-      <c r="Y7">
-        <v>88.1</v>
-      </c>
-      <c r="Z7">
-        <v>-2.4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J7" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>38</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>77</v>
+      <c r="G8" t="s">
+        <v>40</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
-      <c r="J8" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="K8" s="3">
-        <v>-173.9</v>
-      </c>
-      <c r="L8" s="3">
-        <v>6</v>
-      </c>
-      <c r="M8" s="3">
-        <v>71</v>
-      </c>
-      <c r="N8" s="3">
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>-161.5</v>
+      </c>
+      <c r="L8">
+        <v>4.8</v>
+      </c>
+      <c r="M8">
+        <v>55</v>
+      </c>
+      <c r="N8">
+        <v>0.8</v>
+      </c>
+      <c r="O8">
         <v>0.6</v>
       </c>
-      <c r="O8" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="P8" s="3">
-        <v>-108.1</v>
-      </c>
-      <c r="Q8" s="3">
+      <c r="P8">
+        <v>-86.1</v>
+      </c>
+      <c r="Q8">
         <v>2.9</v>
       </c>
-      <c r="R8" s="3">
-        <v>-194.3</v>
-      </c>
-      <c r="S8" s="3">
-        <v>13.8</v>
-      </c>
-      <c r="T8" s="3">
-        <v>-43.6</v>
-      </c>
-      <c r="U8" s="3">
-        <v>3.4</v>
-      </c>
-      <c r="V8" s="3">
-        <v>166</v>
-      </c>
-      <c r="W8" s="3">
-        <v>34.700000000000003</v>
-      </c>
-      <c r="X8" s="3">
-        <v>2677.4</v>
-      </c>
-      <c r="Y8" s="3">
-        <v>64.8</v>
-      </c>
-      <c r="Z8" s="3">
-        <v>-2.2000000000000002</v>
+      <c r="R8">
+        <v>-248.1</v>
+      </c>
+      <c r="S8">
+        <v>24.3</v>
+      </c>
+      <c r="T8">
+        <v>-41.7</v>
+      </c>
+      <c r="U8">
+        <v>2.8</v>
+      </c>
+      <c r="V8">
+        <v>159.1</v>
+      </c>
+      <c r="W8">
+        <v>14.7</v>
+      </c>
+      <c r="X8">
+        <v>2489.8000000000002</v>
+      </c>
+      <c r="Y8">
+        <v>88.1</v>
+      </c>
+      <c r="Z8">
+        <v>-2.4</v>
       </c>
     </row>
     <row r="9" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1392,19 +1365,19 @@
         <v>38</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>46</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
@@ -1412,55 +1385,55 @@
         <v>1</v>
       </c>
       <c r="K9" s="3">
-        <v>-151.30000000000001</v>
+        <v>-173.9</v>
       </c>
       <c r="L9" s="3">
-        <v>8.3000000000000007</v>
+        <v>6</v>
       </c>
       <c r="M9" s="3">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="N9" s="3">
-        <v>16.2</v>
+        <v>0.6</v>
       </c>
       <c r="O9" s="3">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="P9" s="3">
-        <v>-86.8</v>
+        <v>-108.1</v>
       </c>
       <c r="Q9" s="3">
-        <v>4.5</v>
+        <v>2.9</v>
       </c>
       <c r="R9" s="3">
-        <v>-235.4</v>
+        <v>-194.3</v>
       </c>
       <c r="S9" s="3">
-        <v>9.4</v>
+        <v>13.8</v>
       </c>
       <c r="T9" s="3">
-        <v>-29</v>
+        <v>-43.6</v>
       </c>
       <c r="U9" s="3">
-        <v>3.7</v>
+        <v>3.4</v>
       </c>
       <c r="V9" s="3">
-        <v>113.6</v>
+        <v>166</v>
       </c>
       <c r="W9" s="3">
-        <v>66.3</v>
+        <v>34.700000000000003</v>
       </c>
       <c r="X9" s="3">
-        <v>2304.4</v>
+        <v>2677.4</v>
       </c>
       <c r="Y9" s="3">
-        <v>21.1</v>
+        <v>64.8</v>
       </c>
       <c r="Z9" s="3">
-        <v>-1.6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+        <v>-2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>33</v>
       </c>
@@ -1468,75 +1441,75 @@
         <v>38</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G10" t="s">
-        <v>41</v>
+        <v>46</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
-      <c r="J10" t="b">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>-159.4</v>
-      </c>
-      <c r="L10">
-        <v>3.4</v>
-      </c>
-      <c r="M10">
-        <v>38</v>
-      </c>
-      <c r="N10">
-        <v>0.7</v>
-      </c>
-      <c r="O10">
-        <v>0.4</v>
-      </c>
-      <c r="P10">
-        <v>-93.1</v>
-      </c>
-      <c r="Q10">
-        <v>6.4</v>
-      </c>
-      <c r="R10">
-        <v>-194.1</v>
-      </c>
-      <c r="S10">
-        <v>30</v>
-      </c>
-      <c r="T10">
-        <v>-37.9</v>
-      </c>
-      <c r="U10">
-        <v>7.2</v>
-      </c>
-      <c r="V10">
-        <v>104.7</v>
-      </c>
-      <c r="W10">
-        <v>51.7</v>
-      </c>
-      <c r="X10">
-        <v>2416.6999999999998</v>
-      </c>
-      <c r="Y10">
-        <v>101.2</v>
-      </c>
-      <c r="Z10">
-        <v>-2.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J10" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" s="3">
+        <v>-151.30000000000001</v>
+      </c>
+      <c r="L10" s="3">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="M10" s="3">
+        <v>68</v>
+      </c>
+      <c r="N10" s="3">
+        <v>16.2</v>
+      </c>
+      <c r="O10" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="P10" s="3">
+        <v>-86.8</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="R10" s="3">
+        <v>-235.4</v>
+      </c>
+      <c r="S10" s="3">
+        <v>9.4</v>
+      </c>
+      <c r="T10" s="3">
+        <v>-29</v>
+      </c>
+      <c r="U10" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="V10" s="3">
+        <v>113.6</v>
+      </c>
+      <c r="W10" s="3">
+        <v>66.3</v>
+      </c>
+      <c r="X10" s="3">
+        <v>2304.4</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>21.1</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>33</v>
       </c>
@@ -1547,300 +1520,252 @@
         <v>67</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
+      </c>
+      <c r="G11" t="s">
+        <v>41</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
-      <c r="J11" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="K11" s="3">
-        <v>-87.4</v>
-      </c>
-      <c r="L11" s="3">
-        <v>3.9</v>
-      </c>
-      <c r="M11" s="3">
-        <v>24</v>
-      </c>
-      <c r="N11" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="O11" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="P11" s="3">
-        <v>-48.1</v>
-      </c>
-      <c r="Q11" s="3">
-        <v>4.8</v>
-      </c>
-      <c r="R11" s="3">
-        <v>-189.2</v>
-      </c>
-      <c r="S11" s="3">
-        <v>10.4</v>
-      </c>
-      <c r="T11" s="3">
-        <v>-23.5</v>
-      </c>
-      <c r="U11" s="3">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="V11" s="3">
-        <v>221.4</v>
-      </c>
-      <c r="W11" s="3">
-        <v>61.7</v>
-      </c>
-      <c r="X11" s="3">
-        <v>1420.6</v>
-      </c>
-      <c r="Y11" s="3">
-        <v>10.5</v>
-      </c>
-      <c r="Z11" s="3">
-        <v>-2.1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" t="s">
-        <v>52</v>
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>-159.4</v>
+      </c>
+      <c r="L11">
+        <v>3.4</v>
+      </c>
+      <c r="M11">
+        <v>38</v>
+      </c>
+      <c r="N11">
+        <v>0.7</v>
+      </c>
+      <c r="O11">
+        <v>0.4</v>
+      </c>
+      <c r="P11">
+        <v>-93.1</v>
+      </c>
+      <c r="Q11">
+        <v>6.4</v>
+      </c>
+      <c r="R11">
+        <v>-194.1</v>
+      </c>
+      <c r="S11">
+        <v>30</v>
+      </c>
+      <c r="T11">
+        <v>-37.9</v>
+      </c>
+      <c r="U11">
+        <v>7.2</v>
+      </c>
+      <c r="V11">
+        <v>104.7</v>
+      </c>
+      <c r="W11">
+        <v>51.7</v>
+      </c>
+      <c r="X11">
+        <v>2416.6999999999998</v>
+      </c>
+      <c r="Y11">
+        <v>101.2</v>
+      </c>
+      <c r="Z11">
+        <v>-2.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" t="s">
-        <v>51</v>
+        <v>67</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" t="s">
-        <v>56</v>
+        <v>91</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
-      <c r="J12" t="b">
-        <v>1</v>
-      </c>
-      <c r="K12">
-        <v>-156</v>
-      </c>
-      <c r="L12">
-        <v>6.3</v>
-      </c>
-      <c r="M12">
-        <v>50</v>
-      </c>
-      <c r="N12">
+      <c r="J12" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" s="3">
+        <v>-87.4</v>
+      </c>
+      <c r="L12" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="M12" s="3">
+        <v>24</v>
+      </c>
+      <c r="N12" s="3">
         <v>0.3</v>
       </c>
-      <c r="O12">
-        <v>0.2</v>
-      </c>
-      <c r="P12">
-        <v>-86.1</v>
-      </c>
-      <c r="Q12">
+      <c r="O12" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="P12" s="3">
+        <v>-48.1</v>
+      </c>
+      <c r="Q12" s="3">
         <v>4.8</v>
       </c>
-      <c r="R12">
-        <v>-354.4</v>
-      </c>
-      <c r="S12">
-        <v>12</v>
-      </c>
-      <c r="T12">
-        <v>-13.8</v>
-      </c>
-      <c r="U12">
-        <v>0.5</v>
-      </c>
-      <c r="V12">
-        <v>147.6</v>
-      </c>
-      <c r="W12">
-        <v>26.9</v>
-      </c>
-      <c r="X12">
-        <v>2479</v>
-      </c>
-      <c r="Y12">
-        <v>50.9</v>
-      </c>
-      <c r="Z12">
-        <v>-2.4</v>
+      <c r="R12" s="3">
+        <v>-189.2</v>
+      </c>
+      <c r="S12" s="3">
+        <v>10.4</v>
+      </c>
+      <c r="T12" s="3">
+        <v>-23.5</v>
+      </c>
+      <c r="U12" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="V12" s="3">
+        <v>221.4</v>
+      </c>
+      <c r="W12" s="3">
+        <v>61.7</v>
+      </c>
+      <c r="X12" s="3">
+        <v>1420.6</v>
+      </c>
+      <c r="Y12" s="3">
+        <v>10.5</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>-2.1</v>
       </c>
     </row>
     <row r="13" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>36</v>
+      <c r="A13" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K13" s="3">
-        <v>-148.1</v>
-      </c>
-      <c r="L13" s="3">
-        <v>2.1</v>
-      </c>
-      <c r="M13" s="3">
-        <v>87</v>
-      </c>
-      <c r="N13" s="3">
-        <v>1</v>
-      </c>
-      <c r="O13" s="3">
-        <v>1</v>
-      </c>
-      <c r="P13" s="3">
-        <v>-89.5</v>
-      </c>
-      <c r="Q13" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="R13" s="3">
-        <v>-254.6</v>
-      </c>
-      <c r="S13" s="3">
-        <v>9.6</v>
-      </c>
-      <c r="T13" s="3">
-        <v>-20.6</v>
-      </c>
-      <c r="U13" s="3">
-        <v>2.9</v>
-      </c>
-      <c r="V13" s="3">
-        <v>129.9</v>
-      </c>
-      <c r="W13" s="3">
-        <v>44.6</v>
-      </c>
-      <c r="X13" s="3">
-        <v>2545.9</v>
-      </c>
-      <c r="Y13" s="3">
-        <v>44.4</v>
-      </c>
-      <c r="Z13" s="3">
-        <v>-2.4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" t="s">
         <v>52</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>80</v>
+      <c r="G14" t="s">
+        <v>56</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="K14" s="3">
-        <v>-136.1</v>
-      </c>
-      <c r="L14" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="M14" s="3">
-        <v>76</v>
-      </c>
-      <c r="N14" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="O14" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="P14" s="3">
-        <v>-87.6</v>
-      </c>
-      <c r="Q14" s="3">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="R14" s="3">
-        <v>-231.2</v>
-      </c>
-      <c r="S14" s="3">
-        <v>7.3</v>
-      </c>
-      <c r="T14" s="3">
-        <v>-15.4</v>
-      </c>
-      <c r="U14" s="3">
-        <v>1</v>
-      </c>
-      <c r="V14" s="3">
-        <v>131.5</v>
-      </c>
-      <c r="W14" s="3">
-        <v>26.4</v>
-      </c>
-      <c r="X14" s="3">
-        <v>2385.3000000000002</v>
-      </c>
-      <c r="Y14" s="3">
-        <v>104.2</v>
-      </c>
-      <c r="Z14" s="3">
-        <v>-2.1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>-156</v>
+      </c>
+      <c r="L14">
+        <v>6.3</v>
+      </c>
+      <c r="M14">
+        <v>50</v>
+      </c>
+      <c r="N14">
+        <v>0.3</v>
+      </c>
+      <c r="O14">
+        <v>0.2</v>
+      </c>
+      <c r="P14">
+        <v>-86.1</v>
+      </c>
+      <c r="Q14">
+        <v>4.8</v>
+      </c>
+      <c r="R14">
+        <v>-354.4</v>
+      </c>
+      <c r="S14">
+        <v>12</v>
+      </c>
+      <c r="T14">
+        <v>-13.8</v>
+      </c>
+      <c r="U14">
+        <v>0.5</v>
+      </c>
+      <c r="V14">
+        <v>147.6</v>
+      </c>
+      <c r="W14">
+        <v>26.9</v>
+      </c>
+      <c r="X14">
+        <v>2479</v>
+      </c>
+      <c r="Y14">
+        <v>50.9</v>
+      </c>
+      <c r="Z14">
+        <v>-2.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>36</v>
       </c>
@@ -1848,75 +1773,75 @@
         <v>52</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
-      <c r="J15" t="b">
-        <v>1</v>
-      </c>
-      <c r="K15">
-        <v>-99.6</v>
-      </c>
-      <c r="L15">
-        <v>4.7</v>
-      </c>
-      <c r="M15">
-        <v>16</v>
-      </c>
-      <c r="N15">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="O15">
-        <v>0.5</v>
-      </c>
-      <c r="P15">
-        <v>-61.7</v>
-      </c>
-      <c r="Q15">
-        <v>2.5</v>
-      </c>
-      <c r="R15">
-        <v>-171.8</v>
-      </c>
-      <c r="S15">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="T15">
-        <v>-19.5</v>
-      </c>
-      <c r="U15">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="V15">
-        <v>159.4</v>
-      </c>
-      <c r="W15">
-        <v>31.8</v>
-      </c>
-      <c r="X15">
-        <v>1992.6</v>
-      </c>
-      <c r="Y15">
-        <v>123.4</v>
-      </c>
-      <c r="Z15">
-        <v>-1.6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J15" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15" s="3">
+        <v>-148.1</v>
+      </c>
+      <c r="L15" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="M15" s="3">
+        <v>87</v>
+      </c>
+      <c r="N15" s="3">
+        <v>1</v>
+      </c>
+      <c r="O15" s="3">
+        <v>1</v>
+      </c>
+      <c r="P15" s="3">
+        <v>-89.5</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="R15" s="3">
+        <v>-254.6</v>
+      </c>
+      <c r="S15" s="3">
+        <v>9.6</v>
+      </c>
+      <c r="T15" s="3">
+        <v>-20.6</v>
+      </c>
+      <c r="U15" s="3">
+        <v>2.9</v>
+      </c>
+      <c r="V15" s="3">
+        <v>129.9</v>
+      </c>
+      <c r="W15" s="3">
+        <v>44.6</v>
+      </c>
+      <c r="X15" s="3">
+        <v>2545.9</v>
+      </c>
+      <c r="Y15" s="3">
+        <v>44.4</v>
+      </c>
+      <c r="Z15" s="3">
+        <v>-2.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>36</v>
       </c>
@@ -1924,19 +1849,19 @@
         <v>52</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
@@ -1944,359 +1869,311 @@
         <v>1</v>
       </c>
       <c r="K16" s="3">
-        <v>-43.9</v>
+        <v>-136.1</v>
       </c>
       <c r="L16" s="3">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="M16" s="3">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="N16" s="3">
-        <v>11.5</v>
+        <v>0.8</v>
       </c>
       <c r="O16" s="3">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="P16" s="3">
-        <v>-41.1</v>
+        <v>-87.6</v>
       </c>
       <c r="Q16" s="3">
-        <v>4.7</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="R16" s="3">
-        <v>-207.9</v>
+        <v>-231.2</v>
       </c>
       <c r="S16" s="3">
-        <v>33.9</v>
+        <v>7.3</v>
       </c>
       <c r="T16" s="3">
-        <v>10.199999999999999</v>
+        <v>-15.4</v>
       </c>
       <c r="U16" s="3">
-        <v>2.2000000000000002</v>
+        <v>1</v>
       </c>
       <c r="V16" s="3">
-        <v>286</v>
+        <v>131.5</v>
       </c>
       <c r="W16" s="3">
-        <v>42.5</v>
+        <v>26.4</v>
       </c>
       <c r="X16" s="3">
-        <v>1600.2</v>
+        <v>2385.3000000000002</v>
       </c>
       <c r="Y16" s="3">
-        <v>74.5</v>
+        <v>104.2</v>
       </c>
       <c r="Z16" s="3">
-        <v>-1.7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>55</v>
+        <v>-2.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" t="s">
-        <v>54</v>
+        <v>67</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="3" t="b">
+      <c r="J17" t="b">
         <v>1</v>
       </c>
       <c r="K17">
-        <v>-144.4</v>
+        <v>-99.6</v>
       </c>
       <c r="L17">
-        <v>1.1000000000000001</v>
+        <v>4.7</v>
       </c>
       <c r="M17">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="N17">
-        <v>1.8</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="O17">
-        <v>1.4</v>
+        <v>0.5</v>
       </c>
       <c r="P17">
-        <v>-85</v>
+        <v>-61.7</v>
       </c>
       <c r="Q17">
-        <v>5.6</v>
+        <v>2.5</v>
       </c>
       <c r="R17">
-        <v>-280.89999999999998</v>
+        <v>-171.8</v>
       </c>
       <c r="S17">
-        <v>23.9</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="T17">
-        <v>-18.899999999999999</v>
+        <v>-19.5</v>
       </c>
       <c r="U17">
-        <v>3.2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="V17">
-        <v>154.1</v>
+        <v>159.4</v>
       </c>
       <c r="W17">
-        <v>39.700000000000003</v>
+        <v>31.8</v>
       </c>
       <c r="X17">
-        <v>2417.8000000000002</v>
+        <v>1992.6</v>
       </c>
       <c r="Y17">
-        <v>163.9</v>
+        <v>123.4</v>
       </c>
       <c r="Z17">
-        <v>-2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>32</v>
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
-      <c r="J18" s="4" t="b">
+      <c r="J18" s="3" t="b">
         <v>1</v>
       </c>
       <c r="K18" s="3">
-        <v>-139.6</v>
+        <v>-43.9</v>
       </c>
       <c r="L18" s="3">
-        <v>4.5</v>
+        <v>1</v>
       </c>
       <c r="M18" s="3">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="N18" s="3">
-        <v>8.5</v>
+        <v>11.5</v>
       </c>
       <c r="O18" s="3">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="P18" s="3">
-        <v>-78.599999999999994</v>
+        <v>-41.1</v>
       </c>
       <c r="Q18" s="3">
-        <v>9.6999999999999993</v>
+        <v>4.7</v>
       </c>
       <c r="R18" s="3">
-        <v>-256.10000000000002</v>
+        <v>-207.9</v>
       </c>
       <c r="S18" s="3">
-        <v>61.8</v>
+        <v>33.9</v>
       </c>
       <c r="T18" s="3">
-        <v>-31.9</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="U18" s="3">
-        <v>6.3</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="V18" s="3">
-        <v>221.4</v>
+        <v>286</v>
       </c>
       <c r="W18" s="3">
-        <v>43.9</v>
+        <v>42.5</v>
       </c>
       <c r="X18" s="3">
-        <v>2407.5</v>
+        <v>1600.2</v>
       </c>
       <c r="Y18" s="3">
-        <v>137.6</v>
+        <v>74.5</v>
       </c>
       <c r="Z18" s="3">
-        <v>-1.8</v>
+        <v>-1.7</v>
       </c>
     </row>
     <row r="19" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>32</v>
+      <c r="A19" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K19" s="3">
-        <v>-174.1</v>
-      </c>
-      <c r="L19" s="3">
-        <v>7.2</v>
-      </c>
-      <c r="M19" s="3">
-        <v>42</v>
-      </c>
-      <c r="N19" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="O19" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="P19" s="3">
-        <v>-95</v>
-      </c>
-      <c r="Q19" s="3">
-        <v>3.2</v>
-      </c>
-      <c r="R19" s="3">
-        <v>-379.8</v>
-      </c>
-      <c r="S19" s="3">
-        <v>61</v>
-      </c>
-      <c r="T19" s="3">
-        <v>-20.8</v>
-      </c>
-      <c r="U19" s="3">
-        <v>6.6</v>
-      </c>
-      <c r="V19" s="3">
-        <v>176.2</v>
-      </c>
-      <c r="W19" s="3">
-        <v>22</v>
-      </c>
-      <c r="X19" s="3">
-        <v>2766.9</v>
-      </c>
-      <c r="Y19" s="3">
-        <v>89.3</v>
-      </c>
-      <c r="Z19" s="3">
-        <v>-1.8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" t="s">
         <v>55</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
+      </c>
+      <c r="D20" t="s">
+        <v>54</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
-      <c r="J20" t="b">
+      <c r="J20" s="3" t="b">
         <v>1</v>
       </c>
       <c r="K20">
-        <v>-126.8</v>
+        <v>-144.4</v>
       </c>
       <c r="L20">
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="M20">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="N20">
-        <v>13.6</v>
+        <v>1.8</v>
       </c>
       <c r="O20">
-        <v>0.8</v>
+        <v>1.4</v>
       </c>
       <c r="P20">
-        <v>-71.8</v>
+        <v>-85</v>
       </c>
       <c r="Q20">
-        <v>4.2</v>
+        <v>5.6</v>
       </c>
       <c r="R20">
-        <v>-268.89999999999998</v>
+        <v>-280.89999999999998</v>
       </c>
       <c r="S20">
-        <v>19.3</v>
+        <v>23.9</v>
       </c>
       <c r="T20">
-        <v>-17.100000000000001</v>
+        <v>-18.899999999999999</v>
       </c>
       <c r="U20">
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="V20">
-        <v>158.80000000000001</v>
+        <v>154.1</v>
       </c>
       <c r="W20">
-        <v>44.7</v>
+        <v>39.700000000000003</v>
       </c>
       <c r="X20">
-        <v>2299.6</v>
+        <v>2417.8000000000002</v>
       </c>
       <c r="Y20">
-        <v>139.69999999999999</v>
+        <v>163.9</v>
       </c>
       <c r="Z20">
-        <v>-2.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>-2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>32</v>
       </c>
@@ -2304,79 +2181,335 @@
         <v>55</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="3" t="b">
+      <c r="J21" s="4" t="b">
         <v>1</v>
       </c>
       <c r="K21" s="3">
+        <v>-139.6</v>
+      </c>
+      <c r="L21" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="M21" s="3">
+        <v>50</v>
+      </c>
+      <c r="N21" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="O21" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="P21" s="3">
+        <v>-78.599999999999994</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="R21" s="3">
+        <v>-256.10000000000002</v>
+      </c>
+      <c r="S21" s="3">
+        <v>61.8</v>
+      </c>
+      <c r="T21" s="3">
+        <v>-31.9</v>
+      </c>
+      <c r="U21" s="3">
+        <v>6.3</v>
+      </c>
+      <c r="V21" s="3">
+        <v>221.4</v>
+      </c>
+      <c r="W21" s="3">
+        <v>43.9</v>
+      </c>
+      <c r="X21" s="3">
+        <v>2407.5</v>
+      </c>
+      <c r="Y21" s="3">
+        <v>137.6</v>
+      </c>
+      <c r="Z21" s="3">
+        <v>-1.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K22" s="3">
+        <v>-174.1</v>
+      </c>
+      <c r="L22" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="M22" s="3">
+        <v>42</v>
+      </c>
+      <c r="N22" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="O22" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="P22" s="3">
+        <v>-95</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="R22" s="3">
+        <v>-379.8</v>
+      </c>
+      <c r="S22" s="3">
+        <v>61</v>
+      </c>
+      <c r="T22" s="3">
+        <v>-20.8</v>
+      </c>
+      <c r="U22" s="3">
+        <v>6.6</v>
+      </c>
+      <c r="V22" s="3">
+        <v>176.2</v>
+      </c>
+      <c r="W22" s="3">
+        <v>22</v>
+      </c>
+      <c r="X22" s="3">
+        <v>2766.9</v>
+      </c>
+      <c r="Y22" s="3">
+        <v>89.3</v>
+      </c>
+      <c r="Z22" s="3">
+        <v>-1.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" t="b">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>-126.8</v>
+      </c>
+      <c r="L23">
+        <v>1.2</v>
+      </c>
+      <c r="M23">
+        <v>26</v>
+      </c>
+      <c r="N23">
+        <v>13.6</v>
+      </c>
+      <c r="O23">
+        <v>0.8</v>
+      </c>
+      <c r="P23">
+        <v>-71.8</v>
+      </c>
+      <c r="Q23">
+        <v>4.2</v>
+      </c>
+      <c r="R23">
+        <v>-268.89999999999998</v>
+      </c>
+      <c r="S23">
+        <v>19.3</v>
+      </c>
+      <c r="T23">
+        <v>-17.100000000000001</v>
+      </c>
+      <c r="U23">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="V23">
+        <v>158.80000000000001</v>
+      </c>
+      <c r="W23">
+        <v>44.7</v>
+      </c>
+      <c r="X23">
+        <v>2299.6</v>
+      </c>
+      <c r="Y23">
+        <v>139.69999999999999</v>
+      </c>
+      <c r="Z23">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24" s="3">
         <v>-78.400000000000006</v>
       </c>
-      <c r="L21" s="3">
+      <c r="L24" s="3">
         <v>2.5</v>
       </c>
-      <c r="M21" s="3">
+      <c r="M24" s="3">
         <v>36</v>
       </c>
-      <c r="N21" s="3">
+      <c r="N24" s="3">
         <v>0.2</v>
       </c>
-      <c r="O21" s="3">
+      <c r="O24" s="3">
         <v>0.1</v>
       </c>
-      <c r="P21" s="3">
+      <c r="P24" s="3">
         <v>-44.2</v>
       </c>
-      <c r="Q21" s="3">
+      <c r="Q24" s="3">
         <v>3</v>
       </c>
-      <c r="R21" s="3">
+      <c r="R24" s="3">
         <v>-324.5</v>
       </c>
-      <c r="S21" s="3">
+      <c r="S24" s="3">
         <v>15</v>
       </c>
-      <c r="T21" s="3">
+      <c r="T24" s="3">
         <v>-3.2</v>
       </c>
-      <c r="U21" s="3">
+      <c r="U24" s="3">
         <v>0.3</v>
       </c>
-      <c r="V21" s="3">
+      <c r="V24" s="3">
         <v>338.6</v>
       </c>
-      <c r="W21" s="3">
+      <c r="W24" s="3">
         <v>21.2</v>
       </c>
-      <c r="X21" s="3">
+      <c r="X24" s="3">
         <v>1555.1</v>
       </c>
-      <c r="Y21" s="3">
+      <c r="Y24" s="3">
         <v>16.399999999999999</v>
       </c>
-      <c r="Z21" s="3">
+      <c r="Z24" s="3">
         <v>-1.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="3" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:Z5" xr:uid="{30842AB1-A644-42C7-A90C-F34DF0E50414}"/>
   <mergeCells count="2">
-    <mergeCell ref="H2:H21"/>
-    <mergeCell ref="I2:I21"/>
+    <mergeCell ref="H2:H25"/>
+    <mergeCell ref="I2:I25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add 7T9J (actual) Omicron docking prediction results
</commit_message>
<xml_diff>
--- a/docking/HADDOCK_Results.xlsx
+++ b/docking/HADDOCK_Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby\Documents\GitHub\SARS-CoV-2_B.1.1.529_Spike-RBD_Predictions\docking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colbyford/Documents/SARS-CoV-2_B.1.1.529_Spike-RBD_Predictions/docking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B665BA9-D93C-4DD1-9225-B1A38F63729F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7E6444-D739-0F49-B492-6F3D621E87FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{05BB3759-F2AC-475A-81D0-60BB4FF9CDA1}"/>
+    <workbookView xWindow="8220" yWindow="460" windowWidth="20580" windowHeight="15840" xr2:uid="{05BB3759-F2AC-475A-81D0-60BB4FF9CDA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -753,43 +753,43 @@
   <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="G17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
+      <selection pane="bottomRight" activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="4" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="6" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="183.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="177" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -869,7 +869,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
@@ -949,7 +949,7 @@
         <v>-2.5</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>-2.5</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>-2.4</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>-2.6</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>-1.8</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
@@ -1280,8 +1280,56 @@
       <c r="J7" s="3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="K7" s="3">
+        <v>-118.5</v>
+      </c>
+      <c r="L7" s="3">
+        <v>23.8</v>
+      </c>
+      <c r="M7" s="3">
+        <v>5</v>
+      </c>
+      <c r="N7" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="P7" s="3">
+        <v>-76.400000000000006</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="R7" s="3">
+        <v>-169.6</v>
+      </c>
+      <c r="S7" s="3">
+        <v>14.7</v>
+      </c>
+      <c r="T7" s="3">
+        <v>-20.8</v>
+      </c>
+      <c r="U7" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="V7" s="3">
+        <v>125.8</v>
+      </c>
+      <c r="W7" s="3">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="X7" s="3">
+        <v>2121.4</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>257.3</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>-1.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>33</v>
       </c>
@@ -1357,7 +1405,7 @@
         <v>-2.4</v>
       </c>
     </row>
-    <row r="9" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>33</v>
       </c>
@@ -1433,7 +1481,7 @@
         <v>-2.2000000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>33</v>
       </c>
@@ -1509,7 +1557,7 @@
         <v>-1.6</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>33</v>
       </c>
@@ -1585,7 +1633,7 @@
         <v>-2.4</v>
       </c>
     </row>
-    <row r="12" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>33</v>
       </c>
@@ -1661,7 +1709,7 @@
         <v>-2.1</v>
       </c>
     </row>
-    <row r="13" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>33</v>
       </c>
@@ -1688,8 +1736,56 @@
       <c r="J13" s="3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="K13" s="3">
+        <v>-148.9</v>
+      </c>
+      <c r="L13" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M13" s="3">
+        <v>52</v>
+      </c>
+      <c r="N13" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="O13" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="P13" s="3">
+        <v>-94.1</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="R13" s="3">
+        <v>-191.1</v>
+      </c>
+      <c r="S13" s="3">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="T13" s="3">
+        <v>-30.6</v>
+      </c>
+      <c r="U13" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="V13" s="3">
+        <v>140.4</v>
+      </c>
+      <c r="W13" s="3">
+        <v>44.2</v>
+      </c>
+      <c r="X13" s="3">
+        <v>2534.5</v>
+      </c>
+      <c r="Y13" s="3">
+        <v>33.4</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>-2.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>36</v>
       </c>
@@ -1765,7 +1861,7 @@
         <v>-2.4</v>
       </c>
     </row>
-    <row r="15" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>36</v>
       </c>
@@ -1841,7 +1937,7 @@
         <v>-2.4</v>
       </c>
     </row>
-    <row r="16" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>36</v>
       </c>
@@ -1917,7 +2013,7 @@
         <v>-2.1</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>36</v>
       </c>
@@ -1993,7 +2089,7 @@
         <v>-1.6</v>
       </c>
     </row>
-    <row r="18" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>36</v>
       </c>
@@ -2069,7 +2165,7 @@
         <v>-1.7</v>
       </c>
     </row>
-    <row r="19" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>36</v>
       </c>
@@ -2096,8 +2192,56 @@
       <c r="J19" s="3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="K19" s="3">
+        <v>-125.4</v>
+      </c>
+      <c r="L19" s="3">
+        <v>12.6</v>
+      </c>
+      <c r="M19" s="3">
+        <v>12</v>
+      </c>
+      <c r="N19" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="O19" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="P19" s="3">
+        <v>-81.900000000000006</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="R19" s="3">
+        <v>-223.5</v>
+      </c>
+      <c r="S19" s="3">
+        <v>21.4</v>
+      </c>
+      <c r="T19" s="3">
+        <v>-8</v>
+      </c>
+      <c r="U19" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="V19" s="3">
+        <v>92.5</v>
+      </c>
+      <c r="W19" s="3">
+        <v>50.5</v>
+      </c>
+      <c r="X19" s="3">
+        <v>2301.1</v>
+      </c>
+      <c r="Y19" s="3">
+        <v>54.4</v>
+      </c>
+      <c r="Z19" s="3">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>32</v>
       </c>
@@ -2173,7 +2317,7 @@
         <v>-2.2999999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>32</v>
       </c>
@@ -2249,7 +2393,7 @@
         <v>-1.8</v>
       </c>
     </row>
-    <row r="22" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>32</v>
       </c>
@@ -2325,7 +2469,7 @@
         <v>-1.8</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>32</v>
       </c>
@@ -2401,7 +2545,7 @@
         <v>-2.5</v>
       </c>
     </row>
-    <row r="24" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>32</v>
       </c>
@@ -2477,7 +2621,7 @@
         <v>-1.9</v>
       </c>
     </row>
-    <row r="25" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>32</v>
       </c>
@@ -2503,6 +2647,54 @@
       <c r="I25" s="10"/>
       <c r="J25" s="3" t="b">
         <v>1</v>
+      </c>
+      <c r="K25" s="3">
+        <v>-120</v>
+      </c>
+      <c r="L25" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M25" s="3">
+        <v>8</v>
+      </c>
+      <c r="N25" s="3">
+        <v>16.5</v>
+      </c>
+      <c r="O25" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="P25" s="3">
+        <v>-67</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="R25" s="3">
+        <v>-271</v>
+      </c>
+      <c r="S25" s="3">
+        <v>14.7</v>
+      </c>
+      <c r="T25" s="3">
+        <v>-17.2</v>
+      </c>
+      <c r="U25" s="3">
+        <v>5.4</v>
+      </c>
+      <c r="V25" s="3">
+        <v>183.8</v>
+      </c>
+      <c r="W25" s="3">
+        <v>62.5</v>
+      </c>
+      <c r="X25" s="3">
+        <v>1979.8</v>
+      </c>
+      <c r="Y25" s="3">
+        <v>99.6</v>
+      </c>
+      <c r="Z25" s="3">
+        <v>-2</v>
       </c>
     </row>
   </sheetData>
@@ -2525,14 +2717,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -2543,7 +2735,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -2554,7 +2746,7 @@
         <v>5.8999999999999997E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -2565,7 +2757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -2576,7 +2768,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -2587,7 +2779,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -2598,7 +2790,7 @@
         <v>3.3E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2622,13 +2814,13 @@
       <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="145" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>49</v>
       </c>
@@ -2705,7 +2897,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="210" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="224" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>42</v>
       </c>
@@ -2782,7 +2974,7 @@
         <v>-1.6</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
Update comparison figures with 7T9J validation
</commit_message>
<xml_diff>
--- a/docking/HADDOCK_Results.xlsx
+++ b/docking/HADDOCK_Results.xlsx
@@ -1,26 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colbyford/Documents/SARS-CoV-2_B.1.1.529_Spike-RBD_Predictions/docking/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby\Documents\GitHub\SARS-CoV-2_B.1.1.529_Spike-RBD_Predictions\docking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7E6444-D739-0F49-B492-6F3D621E87FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2940511-FF95-4A4F-B5B6-119AE9E9B2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8220" yWindow="460" windowWidth="20580" windowHeight="15840" xr2:uid="{05BB3759-F2AC-475A-81D0-60BB4FF9CDA1}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{05BB3759-F2AC-475A-81D0-60BB4FF9CDA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="wilcox" sheetId="3" r:id="rId2"/>
-    <sheet name="Other Mabs" sheetId="2" r:id="rId3"/>
+    <sheet name="Pct Diff" sheetId="5" r:id="rId2"/>
+    <sheet name="wilcox" sheetId="3" r:id="rId3"/>
+    <sheet name="Other Mabs" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Z$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="3" r:id="rId5"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="109">
   <si>
     <t>Fab PDB</t>
   </si>
@@ -342,6 +346,30 @@
   </si>
   <si>
     <t>Validation</t>
+  </si>
+  <si>
+    <t>Average of HADDOCK score</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Min of HADDOCK score</t>
+  </si>
+  <si>
+    <t>Max of HADDOCK score2</t>
+  </si>
+  <si>
+    <t>AlphaFold2 vs. Ref %diff</t>
+  </si>
+  <si>
+    <t>Validation vs. Ref %diff</t>
+  </si>
+  <si>
+    <t>(All)</t>
   </si>
 </sst>
 </file>
@@ -414,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -436,6 +464,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,6 +484,887 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Colby" refreshedDate="44560.604521759262" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="24" xr:uid="{8E61B887-081A-426B-9165-2C4486BFC57D}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:Z25" sheet="Sheet2"/>
+  </cacheSource>
+  <cacheFields count="26">
+    <cacheField name="Antibody Name" numFmtId="0">
+      <sharedItems count="4">
+        <s v="CC12.1"/>
+        <s v="CC12.3"/>
+        <s v="CV30"/>
+        <s v="C105"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Fab PDB" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Variant" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Spike RBD" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Spike RBD PDB" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Analysis Type" numFmtId="0">
+      <sharedItems count="4">
+        <s v="Reference"/>
+        <s v="AlphaFold2 Prediction"/>
+        <s v="RoseTTAFold Prediction"/>
+        <s v="Validation"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="HADDOCK Job Name" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Fab Active Residues" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="RBD Active Residues" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Submitted" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="HADDOCK score" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-198.6" maxValue="-43.9"/>
+    </cacheField>
+    <cacheField name="HADDOCK score (+/-)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1" maxValue="23.8"/>
+    </cacheField>
+    <cacheField name="Cluster size" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="5" maxValue="109"/>
+    </cacheField>
+    <cacheField name="RMSD from the overall lowest-energy structure" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.2" maxValue="16.5"/>
+    </cacheField>
+    <cacheField name="RMSD from the overall lowest-energy structure (+/-)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.1" maxValue="1.4"/>
+    </cacheField>
+    <cacheField name="Van der Waals energy" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-108.1" maxValue="-27.5"/>
+    </cacheField>
+    <cacheField name="Van der Waals energy (+/-)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="2.1" maxValue="17.399999999999999"/>
+    </cacheField>
+    <cacheField name="Electrostatic energy" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-379.8" maxValue="-169.6"/>
+    </cacheField>
+    <cacheField name="Electrostatic energy (+/-)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="7.3" maxValue="61.8"/>
+    </cacheField>
+    <cacheField name="Desolvation energy" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-43.6" maxValue="10.199999999999999"/>
+    </cacheField>
+    <cacheField name="Desolvation energy (+/-)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.3" maxValue="7.2"/>
+    </cacheField>
+    <cacheField name="Restraints violation energy" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="92.5" maxValue="338.6"/>
+    </cacheField>
+    <cacheField name="Restraints violation energy (+/-)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="14.7" maxValue="66.3"/>
+    </cacheField>
+    <cacheField name="Buried Surface Area" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1420.6" maxValue="2778.5"/>
+    </cacheField>
+    <cacheField name="Surface Area (+/-)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="10.5" maxValue="257.3"/>
+    </cacheField>
+    <cacheField name="Z-Score" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-2.6" maxValue="-1.4"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="24">
+  <r>
+    <x v="0"/>
+    <s v="6xc2_chainsHL_Fab_renumbered.pdb"/>
+    <s v="Alpha"/>
+    <s v="6XC2 Chain A"/>
+    <s v="6xc2_chainA_RBD_renumbered.pdb"/>
+    <x v="0"/>
+    <s v="SRBC_6XC2"/>
+    <s v="2,26,28,31,32,33,52,53,54,73,74,96,97,98,99,527,530,531,532,549,550,551,552,553,565,566,567,568,569,591,592,594"/>
+    <s v="`406,408,420,424,452,456,458,459,480,481,487,489,490,492,496,501,503,504,508"/>
+    <b v="1"/>
+    <n v="-198.6"/>
+    <n v="5.0999999999999996"/>
+    <n v="95"/>
+    <n v="0.3"/>
+    <n v="0.2"/>
+    <n v="-106.9"/>
+    <n v="2.2000000000000002"/>
+    <n v="-342.6"/>
+    <n v="10.1"/>
+    <n v="-37.5"/>
+    <n v="2.2000000000000002"/>
+    <n v="143.19999999999999"/>
+    <n v="32"/>
+    <n v="2778.5"/>
+    <n v="63.1"/>
+    <n v="-2.5"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="6xc2_chainsHL_Fab_renumbered.pdb"/>
+    <s v="Beta"/>
+    <s v="7VX1 Chain A"/>
+    <s v="7vx1_chainA_RBD_renumbered.pdb"/>
+    <x v="0"/>
+    <s v="SRBC_7VX1_CC121"/>
+    <m/>
+    <m/>
+    <b v="1"/>
+    <n v="-171.9"/>
+    <n v="6.1"/>
+    <n v="39"/>
+    <n v="0.4"/>
+    <n v="0.2"/>
+    <n v="-93.9"/>
+    <n v="2.1"/>
+    <n v="-298.10000000000002"/>
+    <n v="13.1"/>
+    <n v="-33.1"/>
+    <n v="2.7"/>
+    <n v="147.30000000000001"/>
+    <n v="41.2"/>
+    <n v="2698.8"/>
+    <n v="81.099999999999994"/>
+    <n v="-2.5"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="6xc2_chainsHL_Fab_renumbered.pdb"/>
+    <s v="Delta"/>
+    <s v="7V7O Chain A"/>
+    <s v="7v7o_chainA_RBD_renumbered.pdb"/>
+    <x v="0"/>
+    <s v="SRBC_7V7O_CC121"/>
+    <m/>
+    <m/>
+    <b v="1"/>
+    <n v="-178.8"/>
+    <n v="2.1"/>
+    <n v="109"/>
+    <n v="0.6"/>
+    <n v="0.3"/>
+    <n v="-100.2"/>
+    <n v="5.7"/>
+    <n v="-290.8"/>
+    <n v="45.7"/>
+    <n v="-33"/>
+    <n v="2.5"/>
+    <n v="125.3"/>
+    <n v="19.399999999999999"/>
+    <n v="2682.3"/>
+    <n v="44.6"/>
+    <n v="-2.4"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="6xc2_chainsHL_Fab_renumbered.pdb"/>
+    <s v="Omicron"/>
+    <s v="AlphaFold2 B.1.1.529 Prediction"/>
+    <s v="SARSCov2_B11529_Srbd_80403_relaxed_model_1_rank_1_renumbered.pdb"/>
+    <x v="1"/>
+    <s v="SRBC_pred"/>
+    <m/>
+    <m/>
+    <b v="1"/>
+    <n v="-163.30000000000001"/>
+    <n v="5.0999999999999996"/>
+    <n v="51"/>
+    <n v="0.7"/>
+    <n v="0.5"/>
+    <n v="-90.7"/>
+    <n v="4.4000000000000004"/>
+    <n v="-284.89999999999998"/>
+    <n v="24.1"/>
+    <n v="-28.8"/>
+    <n v="2.4"/>
+    <n v="152.6"/>
+    <n v="46.9"/>
+    <n v="2584.3000000000002"/>
+    <n v="68.400000000000006"/>
+    <n v="-2.6"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="6xc2_chainsHL_Fab_renumbered.pdb"/>
+    <s v="Omicron"/>
+    <s v="RoseTTAFold B.1.1.529 Prediction"/>
+    <s v="SARSCov2_B11529_Srbd_80403_mmseqs2_renumbered.pdb"/>
+    <x v="2"/>
+    <s v="SRBC_RFpred_CC121"/>
+    <m/>
+    <m/>
+    <b v="1"/>
+    <n v="-71.599999999999994"/>
+    <n v="4.5"/>
+    <n v="17"/>
+    <n v="0.3"/>
+    <n v="0.2"/>
+    <n v="-27.5"/>
+    <n v="3.2"/>
+    <n v="-259.2"/>
+    <n v="8.5"/>
+    <n v="-12.4"/>
+    <n v="1.3"/>
+    <n v="201.4"/>
+    <n v="25.7"/>
+    <n v="1578.4"/>
+    <n v="53.3"/>
+    <n v="-1.8"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="6xc2_chainsHL_Fab_renumbered.pdb"/>
+    <s v="Omicron"/>
+    <s v="7T9J Chain C"/>
+    <s v="7t9j_chainC_RBD_renumbered.pdb"/>
+    <x v="3"/>
+    <s v="SRBC_7T9J_CC121"/>
+    <m/>
+    <m/>
+    <b v="1"/>
+    <n v="-118.5"/>
+    <n v="23.8"/>
+    <n v="5"/>
+    <n v="1.2"/>
+    <n v="0.8"/>
+    <n v="-76.400000000000006"/>
+    <n v="17.399999999999999"/>
+    <n v="-169.6"/>
+    <n v="14.7"/>
+    <n v="-20.8"/>
+    <n v="4.3"/>
+    <n v="125.8"/>
+    <n v="17.899999999999999"/>
+    <n v="2121.4"/>
+    <n v="257.3"/>
+    <n v="-1.4"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="6xc7_chainsCD_Fab_renumbered.pdb"/>
+    <s v="Alpha"/>
+    <s v="6XC7 Chain A"/>
+    <s v="6xc7_chainA_RBD_renumbered.pdb"/>
+    <x v="0"/>
+    <s v="SRBC_6XC7_CC123"/>
+    <m/>
+    <m/>
+    <b v="1"/>
+    <n v="-161.5"/>
+    <n v="4.8"/>
+    <n v="55"/>
+    <n v="0.8"/>
+    <n v="0.6"/>
+    <n v="-86.1"/>
+    <n v="2.9"/>
+    <n v="-248.1"/>
+    <n v="24.3"/>
+    <n v="-41.7"/>
+    <n v="2.8"/>
+    <n v="159.1"/>
+    <n v="14.7"/>
+    <n v="2489.8000000000002"/>
+    <n v="88.1"/>
+    <n v="-2.4"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="6xc7_chainsCD_Fab_renumbered.pdb"/>
+    <s v="Beta"/>
+    <s v="7VX1 Chain A"/>
+    <s v="7vx1_chainA_RBD_renumbered.pdb"/>
+    <x v="0"/>
+    <s v="SRBC_7VX1_CC123"/>
+    <m/>
+    <m/>
+    <b v="1"/>
+    <n v="-173.9"/>
+    <n v="6"/>
+    <n v="71"/>
+    <n v="0.6"/>
+    <n v="0.4"/>
+    <n v="-108.1"/>
+    <n v="2.9"/>
+    <n v="-194.3"/>
+    <n v="13.8"/>
+    <n v="-43.6"/>
+    <n v="3.4"/>
+    <n v="166"/>
+    <n v="34.700000000000003"/>
+    <n v="2677.4"/>
+    <n v="64.8"/>
+    <n v="-2.2000000000000002"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="6xc7_chainsCD_Fab_renumbered.pdb"/>
+    <s v="Delta"/>
+    <s v="7V7O Chain A"/>
+    <s v="7v7o_chainA_RBD_renumbered.pdb"/>
+    <x v="0"/>
+    <s v="SRBC_7V7O_CC123"/>
+    <m/>
+    <m/>
+    <b v="1"/>
+    <n v="-151.30000000000001"/>
+    <n v="8.3000000000000007"/>
+    <n v="68"/>
+    <n v="16.2"/>
+    <n v="0.3"/>
+    <n v="-86.8"/>
+    <n v="4.5"/>
+    <n v="-235.4"/>
+    <n v="9.4"/>
+    <n v="-29"/>
+    <n v="3.7"/>
+    <n v="113.6"/>
+    <n v="66.3"/>
+    <n v="2304.4"/>
+    <n v="21.1"/>
+    <n v="-1.6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="6xc7_chainsCD_Fab_renumbered.pdb"/>
+    <s v="Omicron"/>
+    <s v="AlphaFold2 B.1.1.529 Prediction"/>
+    <s v="SARSCov2_B11529_Srbd_80403_relaxed_model_1_rank_1_renumbered.pdb"/>
+    <x v="1"/>
+    <s v="SRBC_pred_CC123"/>
+    <m/>
+    <m/>
+    <b v="1"/>
+    <n v="-159.4"/>
+    <n v="3.4"/>
+    <n v="38"/>
+    <n v="0.7"/>
+    <n v="0.4"/>
+    <n v="-93.1"/>
+    <n v="6.4"/>
+    <n v="-194.1"/>
+    <n v="30"/>
+    <n v="-37.9"/>
+    <n v="7.2"/>
+    <n v="104.7"/>
+    <n v="51.7"/>
+    <n v="2416.6999999999998"/>
+    <n v="101.2"/>
+    <n v="-2.4"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="6xc7_chainsCD_Fab_renumbered.pdb"/>
+    <s v="Omicron"/>
+    <s v="RoseTTAFold B.1.1.529 Prediction"/>
+    <s v="SARSCov2_B11529_Srbd_80403_mmseqs2_renumbered.pdb"/>
+    <x v="2"/>
+    <s v="SRBC_RFpred_CC123"/>
+    <m/>
+    <m/>
+    <b v="1"/>
+    <n v="-87.4"/>
+    <n v="3.9"/>
+    <n v="24"/>
+    <n v="0.3"/>
+    <n v="0.3"/>
+    <n v="-48.1"/>
+    <n v="4.8"/>
+    <n v="-189.2"/>
+    <n v="10.4"/>
+    <n v="-23.5"/>
+    <n v="2.2999999999999998"/>
+    <n v="221.4"/>
+    <n v="61.7"/>
+    <n v="1420.6"/>
+    <n v="10.5"/>
+    <n v="-2.1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="6xc7_chainsCD_Fab_renumbered.pdb"/>
+    <s v="Omicron"/>
+    <s v="7T9J Chain C"/>
+    <s v="7t9j_chainC_RBD_renumbered.pdb"/>
+    <x v="3"/>
+    <s v="SRBC_7T9J_CC123"/>
+    <m/>
+    <m/>
+    <b v="1"/>
+    <n v="-148.9"/>
+    <n v="1.1000000000000001"/>
+    <n v="52"/>
+    <n v="0.6"/>
+    <n v="0.4"/>
+    <n v="-94.1"/>
+    <n v="3.4"/>
+    <n v="-191.1"/>
+    <n v="19.899999999999999"/>
+    <n v="-30.6"/>
+    <n v="2.8"/>
+    <n v="140.4"/>
+    <n v="44.2"/>
+    <n v="2534.5"/>
+    <n v="33.4"/>
+    <n v="-2.1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="6xe1_chainsHL_Fab_renumbered.pdb"/>
+    <s v="Alpha"/>
+    <s v="6XE1 Chain B"/>
+    <s v="6xe1_chainB_RBD_renumbered.pdb"/>
+    <x v="0"/>
+    <s v="SRBC_6XE1_CV30"/>
+    <m/>
+    <m/>
+    <b v="1"/>
+    <n v="-156"/>
+    <n v="6.3"/>
+    <n v="50"/>
+    <n v="0.3"/>
+    <n v="0.2"/>
+    <n v="-86.1"/>
+    <n v="4.8"/>
+    <n v="-354.4"/>
+    <n v="12"/>
+    <n v="-13.8"/>
+    <n v="0.5"/>
+    <n v="147.6"/>
+    <n v="26.9"/>
+    <n v="2479"/>
+    <n v="50.9"/>
+    <n v="-2.4"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="6xe1_chainsHL_Fab_renumbered.pdb"/>
+    <s v="Beta"/>
+    <s v="7VX1 Chain A"/>
+    <s v="7vx1_chainA_RBD_renumbered.pdb"/>
+    <x v="0"/>
+    <s v="SRBC_7VX1_CV30"/>
+    <m/>
+    <m/>
+    <b v="1"/>
+    <n v="-148.1"/>
+    <n v="2.1"/>
+    <n v="87"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="-89.5"/>
+    <n v="4.5"/>
+    <n v="-254.6"/>
+    <n v="9.6"/>
+    <n v="-20.6"/>
+    <n v="2.9"/>
+    <n v="129.9"/>
+    <n v="44.6"/>
+    <n v="2545.9"/>
+    <n v="44.4"/>
+    <n v="-2.4"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="6xe1_chainsHL_Fab_renumbered.pdb"/>
+    <s v="Delta"/>
+    <s v="7V7O Chain A"/>
+    <s v="7v7o_chainA_RBD_renumbered.pdb"/>
+    <x v="0"/>
+    <s v="SRBC_7V7O_CV30"/>
+    <m/>
+    <m/>
+    <b v="1"/>
+    <n v="-136.1"/>
+    <n v="1.5"/>
+    <n v="76"/>
+    <n v="0.8"/>
+    <n v="0.6"/>
+    <n v="-87.6"/>
+    <n v="4.0999999999999996"/>
+    <n v="-231.2"/>
+    <n v="7.3"/>
+    <n v="-15.4"/>
+    <n v="1"/>
+    <n v="131.5"/>
+    <n v="26.4"/>
+    <n v="2385.3000000000002"/>
+    <n v="104.2"/>
+    <n v="-2.1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="6xe1_chainsHL_Fab_renumbered.pdb"/>
+    <s v="Omicron"/>
+    <s v="AlphaFold2 B.1.1.529 Prediction"/>
+    <s v="SARSCov2_B11529_Srbd_80403_relaxed_model_1_rank_1_renumbered.pdb"/>
+    <x v="1"/>
+    <s v="SRBC_pred_CV30"/>
+    <m/>
+    <m/>
+    <b v="1"/>
+    <n v="-99.6"/>
+    <n v="4.7"/>
+    <n v="16"/>
+    <n v="16.100000000000001"/>
+    <n v="0.5"/>
+    <n v="-61.7"/>
+    <n v="2.5"/>
+    <n v="-171.8"/>
+    <n v="16.899999999999999"/>
+    <n v="-19.5"/>
+    <n v="4.4000000000000004"/>
+    <n v="159.4"/>
+    <n v="31.8"/>
+    <n v="1992.6"/>
+    <n v="123.4"/>
+    <n v="-1.6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="6xe1_chainsHL_Fab_renumbered.pdb"/>
+    <s v="Omicron"/>
+    <s v="RoseTTAFold B.1.1.529 Prediction"/>
+    <s v="SARSCov2_B11529_Srbd_80403_mmseqs2_renumbered.pdb"/>
+    <x v="2"/>
+    <s v="SRBC_RFpred_CV30"/>
+    <m/>
+    <m/>
+    <b v="1"/>
+    <n v="-43.9"/>
+    <n v="1"/>
+    <n v="43"/>
+    <n v="11.5"/>
+    <n v="0.2"/>
+    <n v="-41.1"/>
+    <n v="4.7"/>
+    <n v="-207.9"/>
+    <n v="33.9"/>
+    <n v="10.199999999999999"/>
+    <n v="2.2000000000000002"/>
+    <n v="286"/>
+    <n v="42.5"/>
+    <n v="1600.2"/>
+    <n v="74.5"/>
+    <n v="-1.7"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="6xe1_chainsHL_Fab_renumbered.pdb"/>
+    <s v="Omicron"/>
+    <s v="7T9J Chain C"/>
+    <s v="7t9j_chainC_RBD_renumbered.pdb"/>
+    <x v="3"/>
+    <s v="SRBC_7T9J_CV30"/>
+    <m/>
+    <m/>
+    <b v="1"/>
+    <n v="-125.4"/>
+    <n v="12.6"/>
+    <n v="12"/>
+    <n v="0.8"/>
+    <n v="0.6"/>
+    <n v="-81.900000000000006"/>
+    <n v="8.6999999999999993"/>
+    <n v="-223.5"/>
+    <n v="21.4"/>
+    <n v="-8"/>
+    <n v="3.1"/>
+    <n v="92.5"/>
+    <n v="50.5"/>
+    <n v="2301.1"/>
+    <n v="54.4"/>
+    <n v="-1.6"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="6xcm_chainsNS_Fab_renumbered.pdb"/>
+    <s v="Alpha"/>
+    <s v="6XCM Chain B"/>
+    <s v="6xcm_chainB_RBD_renumbered.pdb"/>
+    <x v="0"/>
+    <s v="SRBC_6XCM_C105"/>
+    <m/>
+    <m/>
+    <b v="1"/>
+    <n v="-144.4"/>
+    <n v="1.1000000000000001"/>
+    <n v="73"/>
+    <n v="1.8"/>
+    <n v="1.4"/>
+    <n v="-85"/>
+    <n v="5.6"/>
+    <n v="-280.89999999999998"/>
+    <n v="23.9"/>
+    <n v="-18.899999999999999"/>
+    <n v="3.2"/>
+    <n v="154.1"/>
+    <n v="39.700000000000003"/>
+    <n v="2417.8000000000002"/>
+    <n v="163.9"/>
+    <n v="-2.2999999999999998"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="6xcm_chainsNS_Fab_renumbered.pdb"/>
+    <s v="Beta"/>
+    <s v="7VX1 Chain A"/>
+    <s v="7vx1_chainA_RBD_renumbered.pdb"/>
+    <x v="0"/>
+    <s v="SRBC_7VX1_C105"/>
+    <m/>
+    <m/>
+    <b v="1"/>
+    <n v="-139.6"/>
+    <n v="4.5"/>
+    <n v="50"/>
+    <n v="8.5"/>
+    <n v="0.4"/>
+    <n v="-78.599999999999994"/>
+    <n v="9.6999999999999993"/>
+    <n v="-256.10000000000002"/>
+    <n v="61.8"/>
+    <n v="-31.9"/>
+    <n v="6.3"/>
+    <n v="221.4"/>
+    <n v="43.9"/>
+    <n v="2407.5"/>
+    <n v="137.6"/>
+    <n v="-1.8"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="6xcm_chainsNS_Fab_renumbered.pdb"/>
+    <s v="Delta"/>
+    <s v="7V7O Chain A"/>
+    <s v="7v7o_chainA_RBD_renumbered.pdb"/>
+    <x v="0"/>
+    <s v="SRBC_7V7O_C105"/>
+    <m/>
+    <m/>
+    <b v="1"/>
+    <n v="-174.1"/>
+    <n v="7.2"/>
+    <n v="42"/>
+    <n v="0.6"/>
+    <n v="0.4"/>
+    <n v="-95"/>
+    <n v="3.2"/>
+    <n v="-379.8"/>
+    <n v="61"/>
+    <n v="-20.8"/>
+    <n v="6.6"/>
+    <n v="176.2"/>
+    <n v="22"/>
+    <n v="2766.9"/>
+    <n v="89.3"/>
+    <n v="-1.8"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="6xcm_chainsNS_Fab_renumbered.pdb"/>
+    <s v="Omicron"/>
+    <s v="AlphaFold2 B.1.1.529 Prediction"/>
+    <s v="SARSCov2_B11529_Srbd_80403_relaxed_model_1_rank_1_renumbered.pdb"/>
+    <x v="1"/>
+    <s v="SRBC_pred_C105"/>
+    <m/>
+    <m/>
+    <b v="1"/>
+    <n v="-126.8"/>
+    <n v="1.2"/>
+    <n v="26"/>
+    <n v="13.6"/>
+    <n v="0.8"/>
+    <n v="-71.8"/>
+    <n v="4.2"/>
+    <n v="-268.89999999999998"/>
+    <n v="19.3"/>
+    <n v="-17.100000000000001"/>
+    <n v="2.2000000000000002"/>
+    <n v="158.80000000000001"/>
+    <n v="44.7"/>
+    <n v="2299.6"/>
+    <n v="139.69999999999999"/>
+    <n v="-2.5"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="6xcm_chainsNS_Fab_renumbered.pdb"/>
+    <s v="Omicron"/>
+    <s v="RoseTTAFold B.1.1.529 Prediction"/>
+    <s v="SARSCov2_B11529_Srbd_80403_mmseqs2_renumbered.pdb"/>
+    <x v="2"/>
+    <s v="SRBC_RFpred_C105"/>
+    <m/>
+    <m/>
+    <b v="1"/>
+    <n v="-78.400000000000006"/>
+    <n v="2.5"/>
+    <n v="36"/>
+    <n v="0.2"/>
+    <n v="0.1"/>
+    <n v="-44.2"/>
+    <n v="3"/>
+    <n v="-324.5"/>
+    <n v="15"/>
+    <n v="-3.2"/>
+    <n v="0.3"/>
+    <n v="338.6"/>
+    <n v="21.2"/>
+    <n v="1555.1"/>
+    <n v="16.399999999999999"/>
+    <n v="-1.9"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="6xcm_chainsNS_Fab_renumbered.pdb"/>
+    <s v="Omicron"/>
+    <s v="7T9J Chain C"/>
+    <s v="7t9j_chainC_RBD_renumbered.pdb"/>
+    <x v="3"/>
+    <s v="SRBC_7T9J_C105"/>
+    <m/>
+    <m/>
+    <b v="1"/>
+    <n v="-120"/>
+    <n v="4.2"/>
+    <n v="8"/>
+    <n v="16.5"/>
+    <n v="0.2"/>
+    <n v="-67"/>
+    <n v="5.6"/>
+    <n v="-271"/>
+    <n v="14.7"/>
+    <n v="-17.2"/>
+    <n v="5.4"/>
+    <n v="183.8"/>
+    <n v="62.5"/>
+    <n v="1979.8"/>
+    <n v="99.6"/>
+    <n v="-2"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{57793B0D-4E16-464F-8062-7E207F759BF8}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:D8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="26">
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item x="3"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="5"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="0" hier="-1"/>
+  </pageFields>
+  <dataFields count="3">
+    <dataField name="Min of HADDOCK score" fld="10" subtotal="min" baseField="5" baseItem="0"/>
+    <dataField name="Average of HADDOCK score" fld="10" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Max of HADDOCK score2" fld="10" subtotal="max" baseField="5" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -752,44 +1666,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C05FAB-699E-4769-A909-822D635E1B9A}">
   <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="G17" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K26" sqref="K26"/>
+      <selection pane="bottomRight" activeCell="Z25" sqref="A1:Z25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.5" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="19.83203125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="4" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="6" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="177" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="177" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -869,7 +1783,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
@@ -949,7 +1863,7 @@
         <v>-2.5</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
@@ -1025,7 +1939,7 @@
         <v>-2.5</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
@@ -1101,7 +2015,7 @@
         <v>-2.4</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
@@ -1177,7 +2091,7 @@
         <v>-2.6</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1253,7 +2167,7 @@
         <v>-1.8</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
@@ -1329,7 +2243,7 @@
         <v>-1.4</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>33</v>
       </c>
@@ -1405,7 +2319,7 @@
         <v>-2.4</v>
       </c>
     </row>
-    <row r="9" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>33</v>
       </c>
@@ -1481,7 +2395,7 @@
         <v>-2.2000000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>33</v>
       </c>
@@ -1557,7 +2471,7 @@
         <v>-1.6</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>33</v>
       </c>
@@ -1633,7 +2547,7 @@
         <v>-2.4</v>
       </c>
     </row>
-    <row r="12" spans="1:26" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>33</v>
       </c>
@@ -1709,7 +2623,7 @@
         <v>-2.1</v>
       </c>
     </row>
-    <row r="13" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>33</v>
       </c>
@@ -1785,7 +2699,7 @@
         <v>-2.1</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>36</v>
       </c>
@@ -1861,7 +2775,7 @@
         <v>-2.4</v>
       </c>
     </row>
-    <row r="15" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>36</v>
       </c>
@@ -1937,7 +2851,7 @@
         <v>-2.4</v>
       </c>
     </row>
-    <row r="16" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>36</v>
       </c>
@@ -2013,7 +2927,7 @@
         <v>-2.1</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>36</v>
       </c>
@@ -2089,7 +3003,7 @@
         <v>-1.6</v>
       </c>
     </row>
-    <row r="18" spans="1:26" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>36</v>
       </c>
@@ -2165,7 +3079,7 @@
         <v>-1.7</v>
       </c>
     </row>
-    <row r="19" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>36</v>
       </c>
@@ -2241,7 +3155,7 @@
         <v>-1.6</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>32</v>
       </c>
@@ -2317,7 +3231,7 @@
         <v>-2.2999999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>32</v>
       </c>
@@ -2393,7 +3307,7 @@
         <v>-1.8</v>
       </c>
     </row>
-    <row r="22" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>32</v>
       </c>
@@ -2469,7 +3383,7 @@
         <v>-1.8</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>32</v>
       </c>
@@ -2545,7 +3459,7 @@
         <v>-2.5</v>
       </c>
     </row>
-    <row r="24" spans="1:26" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>32</v>
       </c>
@@ -2621,7 +3535,7 @@
         <v>-1.9</v>
       </c>
     </row>
-    <row r="25" spans="1:26" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>32</v>
       </c>
@@ -2710,6 +3624,139 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EB7B74B-0B0F-4759-A970-25E74CC533ED}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="11">
+        <v>-198.6</v>
+      </c>
+      <c r="C4" s="11">
+        <v>-161.19166666666663</v>
+      </c>
+      <c r="D4" s="11">
+        <v>-136.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="11">
+        <v>-163.30000000000001</v>
+      </c>
+      <c r="C5" s="11">
+        <v>-137.27500000000001</v>
+      </c>
+      <c r="D5" s="11">
+        <v>-99.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="11">
+        <v>-87.4</v>
+      </c>
+      <c r="C6" s="11">
+        <v>-70.325000000000003</v>
+      </c>
+      <c r="D6" s="11">
+        <v>-43.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="11">
+        <v>-148.9</v>
+      </c>
+      <c r="C7" s="11">
+        <v>-128.19999999999999</v>
+      </c>
+      <c r="D7" s="11">
+        <v>-118.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="11">
+        <v>-198.6</v>
+      </c>
+      <c r="C8" s="11">
+        <v>-136.56250000000003</v>
+      </c>
+      <c r="D8" s="11">
+        <v>-43.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13">
+        <f>(GETPIVOTDATA("Average of HADDOCK score",$A$3,"Analysis Type","AlphaFold2 Prediction")-GETPIVOTDATA("Average of HADDOCK score",$A$3,"Analysis Type","Reference"))/GETPIVOTDATA("Average of HADDOCK score",$A$3,"Analysis Type","Reference")</f>
+        <v>-0.14837408881765993</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14">
+        <f>(GETPIVOTDATA("Average of HADDOCK score",$A$3,"Analysis Type","Validation")-GETPIVOTDATA("Average of HADDOCK score",$A$3,"Analysis Type","Reference"))/GETPIVOTDATA("Average of HADDOCK score",$A$3,"Analysis Type","Reference")</f>
+        <v>-0.20467352530631228</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A52817E1-C765-4BB4-9067-03EBE5617AA3}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -2717,14 +3764,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -2735,7 +3782,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -2746,7 +3793,7 @@
         <v>5.8999999999999997E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -2757,7 +3804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -2768,7 +3815,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -2779,7 +3826,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -2790,7 +3837,7 @@
         <v>3.3E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2806,7 +3853,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F2AF89-3042-423C-84CB-DB6A0EAC50E4}">
   <dimension ref="A1:Y3"/>
   <sheetViews>
@@ -2814,13 +3861,13 @@
       <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="145" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="143.25" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>49</v>
       </c>
@@ -2897,7 +3944,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="224" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" ht="210" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>42</v>
       </c>
@@ -2974,7 +4021,7 @@
         <v>-1.6</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
Add HADDOCK results for BA.2.75 and BA.5 for CC12.1
</commit_message>
<xml_diff>
--- a/docking/HADDOCK_Results.xlsx
+++ b/docking/HADDOCK_Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby\Documents\GitHub\SARS-CoV-2_B.1.1.529_Spike-RBD_Predictions\docking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2940511-FF95-4A4F-B5B6-119AE9E9B2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8CA26B-8166-41DF-A78F-83397A9115FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{05BB3759-F2AC-475A-81D0-60BB4FF9CDA1}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{05BB3759-F2AC-475A-81D0-60BB4FF9CDA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,11 @@
     <sheet name="Other Mabs" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Z$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AA$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="123">
   <si>
     <t>Fab PDB</t>
   </si>
@@ -370,6 +370,48 @@
   </si>
   <si>
     <t>(All)</t>
+  </si>
+  <si>
+    <t>BA.2.75</t>
+  </si>
+  <si>
+    <t>RBD_BA2_75_renumbered.pdb</t>
+  </si>
+  <si>
+    <t>SRBC_6XC2_BA275</t>
+  </si>
+  <si>
+    <t>BA.5</t>
+  </si>
+  <si>
+    <t>RBD_BA5_renumbered.pdb</t>
+  </si>
+  <si>
+    <t>SRBC_6XC2_BA5</t>
+  </si>
+  <si>
+    <t>AlphaFold2 BA.2.75 Prediction</t>
+  </si>
+  <si>
+    <t>AlphaFold2 BA.5 Prediction</t>
+  </si>
+  <si>
+    <t>Variant ID</t>
+  </si>
+  <si>
+    <t>B.1.1.7</t>
+  </si>
+  <si>
+    <t>Omicron (Subvariant)</t>
+  </si>
+  <si>
+    <t>B.1.1.529</t>
+  </si>
+  <si>
+    <t>B.1.351</t>
+  </si>
+  <si>
+    <t>B.1.617.2</t>
   </si>
 </sst>
 </file>
@@ -461,13 +503,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="45" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1267,7 +1309,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{57793B0D-4E16-464F-8062-7E207F759BF8}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{57793B0D-4E16-464F-8062-7E207F759BF8}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="26">
     <pivotField axis="axisPage" showAll="0">
@@ -1664,46 +1706,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C05FAB-699E-4769-A909-822D635E1B9A}">
-  <dimension ref="A1:Z25"/>
+  <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z25" sqref="A1:Z25"/>
+      <selection pane="bottomRight" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="177" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="177" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1713,77 +1756,80 @@
       <c r="C1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="S1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="T1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="U1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="V1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="W1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="X1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="Y1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="Z1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="AA1" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
@@ -1793,77 +1839,80 @@
       <c r="C2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="I2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="J2" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="J2" t="b">
+      <c r="K2" t="b">
         <v>1</v>
       </c>
-      <c r="K2" s="3">
+      <c r="L2" s="3">
         <v>-198.6</v>
       </c>
-      <c r="L2" s="3">
+      <c r="M2" s="3">
         <v>5.0999999999999996</v>
       </c>
-      <c r="M2" s="3">
+      <c r="N2" s="3">
         <v>95</v>
       </c>
-      <c r="N2" s="3">
+      <c r="O2" s="3">
         <v>0.3</v>
       </c>
-      <c r="O2" s="3">
+      <c r="P2" s="3">
         <v>0.2</v>
       </c>
-      <c r="P2" s="3">
+      <c r="Q2" s="3">
         <v>-106.9</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="R2" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="R2" s="3">
+      <c r="S2" s="3">
         <v>-342.6</v>
       </c>
-      <c r="S2" s="3">
+      <c r="T2" s="3">
         <v>10.1</v>
       </c>
-      <c r="T2" s="3">
+      <c r="U2" s="3">
         <v>-37.5</v>
       </c>
-      <c r="U2" s="3">
+      <c r="V2" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="V2" s="3">
+      <c r="W2" s="3">
         <v>143.19999999999999</v>
       </c>
-      <c r="W2" s="3">
+      <c r="X2" s="3">
         <v>32</v>
       </c>
-      <c r="X2" s="3">
+      <c r="Y2" s="3">
         <v>2778.5</v>
       </c>
-      <c r="Y2" s="3">
+      <c r="Z2" s="3">
         <v>63.1</v>
       </c>
-      <c r="Z2" s="3">
+      <c r="AA2" s="3">
         <v>-2.5</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
@@ -1874,72 +1923,75 @@
         <v>69</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="3" t="b">
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K3" s="3">
+      <c r="L3" s="3">
         <v>-171.9</v>
       </c>
-      <c r="L3" s="3">
+      <c r="M3" s="3">
         <v>6.1</v>
       </c>
-      <c r="M3" s="3">
+      <c r="N3" s="3">
         <v>39</v>
       </c>
-      <c r="N3" s="3">
+      <c r="O3" s="3">
         <v>0.4</v>
       </c>
-      <c r="O3" s="3">
+      <c r="P3" s="3">
         <v>0.2</v>
       </c>
-      <c r="P3" s="3">
+      <c r="Q3" s="3">
         <v>-93.9</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="R3" s="3">
         <v>2.1</v>
       </c>
-      <c r="R3" s="3">
+      <c r="S3" s="3">
         <v>-298.10000000000002</v>
       </c>
-      <c r="S3" s="3">
+      <c r="T3" s="3">
         <v>13.1</v>
       </c>
-      <c r="T3" s="3">
+      <c r="U3" s="3">
         <v>-33.1</v>
       </c>
-      <c r="U3" s="3">
+      <c r="V3" s="3">
         <v>2.7</v>
       </c>
-      <c r="V3" s="3">
+      <c r="W3" s="3">
         <v>147.30000000000001</v>
       </c>
-      <c r="W3" s="3">
+      <c r="X3" s="3">
         <v>41.2</v>
       </c>
-      <c r="X3" s="3">
+      <c r="Y3" s="3">
         <v>2698.8</v>
       </c>
-      <c r="Y3" s="3">
+      <c r="Z3" s="3">
         <v>81.099999999999994</v>
       </c>
-      <c r="Z3" s="3">
+      <c r="AA3" s="3">
         <v>-2.5</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
@@ -1950,72 +2002,75 @@
         <v>72</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="3" t="b">
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L4" s="3">
         <v>-178.8</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="3">
         <v>2.1</v>
       </c>
-      <c r="M4" s="3">
+      <c r="N4" s="3">
         <v>109</v>
       </c>
-      <c r="N4" s="3">
+      <c r="O4" s="3">
         <v>0.6</v>
       </c>
-      <c r="O4" s="3">
+      <c r="P4" s="3">
         <v>0.3</v>
       </c>
-      <c r="P4" s="3">
+      <c r="Q4" s="3">
         <v>-100.2</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="R4" s="3">
         <v>5.7</v>
       </c>
-      <c r="R4" s="3">
+      <c r="S4" s="3">
         <v>-290.8</v>
       </c>
-      <c r="S4" s="3">
+      <c r="T4" s="3">
         <v>45.7</v>
       </c>
-      <c r="T4" s="3">
+      <c r="U4" s="3">
         <v>-33</v>
       </c>
-      <c r="U4" s="3">
+      <c r="V4" s="3">
         <v>2.5</v>
       </c>
-      <c r="V4" s="3">
+      <c r="W4" s="3">
         <v>125.3</v>
       </c>
-      <c r="W4" s="3">
+      <c r="X4" s="3">
         <v>19.399999999999999</v>
       </c>
-      <c r="X4" s="3">
+      <c r="Y4" s="3">
         <v>2682.3</v>
       </c>
-      <c r="Y4" s="3">
+      <c r="Z4" s="3">
         <v>44.6</v>
       </c>
-      <c r="Z4" s="3">
+      <c r="AA4" s="3">
         <v>-2.4</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
@@ -2025,73 +2080,76 @@
       <c r="C5" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" t="b">
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" t="b">
         <v>1</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="3">
         <v>-163.30000000000001</v>
       </c>
-      <c r="L5" s="3">
+      <c r="M5" s="3">
         <v>5.0999999999999996</v>
       </c>
-      <c r="M5" s="3">
+      <c r="N5" s="3">
         <v>51</v>
       </c>
-      <c r="N5" s="3">
+      <c r="O5" s="3">
         <v>0.7</v>
       </c>
-      <c r="O5" s="3">
+      <c r="P5" s="3">
         <v>0.5</v>
       </c>
-      <c r="P5" s="3">
+      <c r="Q5" s="3">
         <v>-90.7</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="R5" s="3">
         <v>4.4000000000000004</v>
       </c>
-      <c r="R5" s="3">
+      <c r="S5" s="3">
         <v>-284.89999999999998</v>
       </c>
-      <c r="S5" s="3">
+      <c r="T5" s="3">
         <v>24.1</v>
       </c>
-      <c r="T5" s="3">
+      <c r="U5" s="3">
         <v>-28.8</v>
       </c>
-      <c r="U5" s="3">
+      <c r="V5" s="3">
         <v>2.4</v>
       </c>
-      <c r="V5" s="3">
+      <c r="W5" s="3">
         <v>152.6</v>
       </c>
-      <c r="W5" s="3">
+      <c r="X5" s="3">
         <v>46.9</v>
       </c>
-      <c r="X5" s="3">
+      <c r="Y5" s="3">
         <v>2584.3000000000002</v>
       </c>
-      <c r="Y5" s="3">
+      <c r="Z5" s="3">
         <v>68.400000000000006</v>
       </c>
-      <c r="Z5" s="3">
+      <c r="AA5" s="3">
         <v>-2.6</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
@@ -2102,72 +2160,75 @@
         <v>67</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="3" t="b">
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K6" s="3">
+      <c r="L6" s="3">
         <v>-71.599999999999994</v>
       </c>
-      <c r="L6" s="3">
+      <c r="M6" s="3">
         <v>4.5</v>
       </c>
-      <c r="M6" s="3">
+      <c r="N6" s="3">
         <v>17</v>
       </c>
-      <c r="N6" s="3">
+      <c r="O6" s="3">
         <v>0.3</v>
       </c>
-      <c r="O6" s="3">
+      <c r="P6" s="3">
         <v>0.2</v>
       </c>
-      <c r="P6" s="3">
+      <c r="Q6" s="3">
         <v>-27.5</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="R6" s="3">
         <v>3.2</v>
       </c>
-      <c r="R6" s="3">
+      <c r="S6" s="3">
         <v>-259.2</v>
       </c>
-      <c r="S6" s="3">
+      <c r="T6" s="3">
         <v>8.5</v>
       </c>
-      <c r="T6" s="3">
+      <c r="U6" s="3">
         <v>-12.4</v>
       </c>
-      <c r="U6" s="3">
+      <c r="V6" s="3">
         <v>1.3</v>
       </c>
-      <c r="V6" s="3">
+      <c r="W6" s="3">
         <v>201.4</v>
       </c>
-      <c r="W6" s="3">
+      <c r="X6" s="3">
         <v>25.7</v>
       </c>
-      <c r="X6" s="3">
+      <c r="Y6" s="3">
         <v>1578.4</v>
       </c>
-      <c r="Y6" s="3">
+      <c r="Z6" s="3">
         <v>53.3</v>
       </c>
-      <c r="Z6" s="3">
+      <c r="AA6" s="3">
         <v>-1.8</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
@@ -2178,300 +2239,312 @@
         <v>67</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="3" t="b">
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K7" s="3">
+      <c r="L7" s="3">
         <v>-118.5</v>
       </c>
-      <c r="L7" s="3">
+      <c r="M7" s="3">
         <v>23.8</v>
       </c>
-      <c r="M7" s="3">
+      <c r="N7" s="3">
         <v>5</v>
       </c>
-      <c r="N7" s="3">
+      <c r="O7" s="3">
         <v>1.2</v>
       </c>
-      <c r="O7" s="3">
+      <c r="P7" s="3">
         <v>0.8</v>
       </c>
-      <c r="P7" s="3">
+      <c r="Q7" s="3">
         <v>-76.400000000000006</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="R7" s="3">
         <v>17.399999999999999</v>
       </c>
-      <c r="R7" s="3">
+      <c r="S7" s="3">
         <v>-169.6</v>
       </c>
-      <c r="S7" s="3">
+      <c r="T7" s="3">
         <v>14.7</v>
       </c>
-      <c r="T7" s="3">
+      <c r="U7" s="3">
         <v>-20.8</v>
       </c>
-      <c r="U7" s="3">
+      <c r="V7" s="3">
         <v>4.3</v>
       </c>
-      <c r="V7" s="3">
+      <c r="W7" s="3">
         <v>125.8</v>
       </c>
-      <c r="W7" s="3">
+      <c r="X7" s="3">
         <v>17.899999999999999</v>
       </c>
-      <c r="X7" s="3">
+      <c r="Y7" s="3">
         <v>2121.4</v>
       </c>
-      <c r="Y7" s="3">
+      <c r="Z7" s="3">
         <v>257.3</v>
       </c>
-      <c r="Z7" s="3">
+      <c r="AA7" s="3">
         <v>-1.4</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
+    <row r="8" spans="1:27" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" t="b">
+        <v>119</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K8">
-        <v>-161.5</v>
-      </c>
-      <c r="L8">
-        <v>4.8</v>
-      </c>
-      <c r="M8">
-        <v>55</v>
-      </c>
-      <c r="N8">
-        <v>0.8</v>
-      </c>
-      <c r="O8">
+      <c r="L8" s="3">
+        <v>-118.8</v>
+      </c>
+      <c r="M8" s="3">
+        <v>10.5</v>
+      </c>
+      <c r="N8" s="3">
+        <v>26</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="P8" s="3">
         <v>0.6</v>
       </c>
-      <c r="P8">
-        <v>-86.1</v>
-      </c>
-      <c r="Q8">
+      <c r="Q8" s="3">
+        <v>-72.3</v>
+      </c>
+      <c r="R8" s="3">
+        <v>8</v>
+      </c>
+      <c r="S8" s="3">
+        <v>-265.7</v>
+      </c>
+      <c r="T8" s="3">
+        <v>48.8</v>
+      </c>
+      <c r="U8" s="3">
+        <v>-8.9</v>
+      </c>
+      <c r="V8" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="W8" s="3">
+        <v>155.69999999999999</v>
+      </c>
+      <c r="X8" s="3">
+        <v>53.5</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>2265.6</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>134.30000000000001</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" s="3">
+        <v>-121.4</v>
+      </c>
+      <c r="M9" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="N9" s="3">
+        <v>18</v>
+      </c>
+      <c r="O9" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="P9" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>-78</v>
+      </c>
+      <c r="R9" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="S9" s="3">
+        <v>-198.3</v>
+      </c>
+      <c r="T9" s="3">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="U9" s="3">
+        <v>-18.600000000000001</v>
+      </c>
+      <c r="V9" s="3">
         <v>2.9</v>
       </c>
-      <c r="R8">
-        <v>-248.1</v>
-      </c>
-      <c r="S8">
-        <v>24.3</v>
-      </c>
-      <c r="T8">
-        <v>-41.7</v>
-      </c>
-      <c r="U8">
-        <v>2.8</v>
-      </c>
-      <c r="V8">
-        <v>159.1</v>
-      </c>
-      <c r="W8">
-        <v>14.7</v>
-      </c>
-      <c r="X8">
-        <v>2489.8000000000002</v>
-      </c>
-      <c r="Y8">
-        <v>88.1</v>
-      </c>
-      <c r="Z8">
-        <v>-2.4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="K9" s="3">
-        <v>-173.9</v>
-      </c>
-      <c r="L9" s="3">
-        <v>6</v>
-      </c>
-      <c r="M9" s="3">
-        <v>71</v>
-      </c>
-      <c r="N9" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="O9" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="P9" s="3">
-        <v>-108.1</v>
-      </c>
-      <c r="Q9" s="3">
-        <v>2.9</v>
-      </c>
-      <c r="R9" s="3">
-        <v>-194.3</v>
-      </c>
-      <c r="S9" s="3">
-        <v>13.8</v>
-      </c>
-      <c r="T9" s="3">
-        <v>-43.6</v>
-      </c>
-      <c r="U9" s="3">
-        <v>3.4</v>
-      </c>
-      <c r="V9" s="3">
-        <v>166</v>
-      </c>
       <c r="W9" s="3">
-        <v>34.700000000000003</v>
+        <v>147.30000000000001</v>
       </c>
       <c r="X9" s="3">
-        <v>2677.4</v>
+        <v>36.6</v>
       </c>
       <c r="Y9" s="3">
-        <v>64.8</v>
+        <v>2326.3000000000002</v>
       </c>
       <c r="Z9" s="3">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="AA9" s="3">
         <v>-2.2000000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>75</v>
+        <v>118</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
       </c>
       <c r="F10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="3" t="b">
+      <c r="H10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" t="b">
         <v>1</v>
       </c>
-      <c r="K10" s="3">
-        <v>-151.30000000000001</v>
-      </c>
-      <c r="L10" s="3">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="M10" s="3">
-        <v>68</v>
-      </c>
-      <c r="N10" s="3">
-        <v>16.2</v>
-      </c>
-      <c r="O10" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="P10" s="3">
-        <v>-86.8</v>
-      </c>
-      <c r="Q10" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="R10" s="3">
-        <v>-235.4</v>
-      </c>
-      <c r="S10" s="3">
-        <v>9.4</v>
-      </c>
-      <c r="T10" s="3">
-        <v>-29</v>
-      </c>
-      <c r="U10" s="3">
-        <v>3.7</v>
-      </c>
-      <c r="V10" s="3">
-        <v>113.6</v>
-      </c>
-      <c r="W10" s="3">
-        <v>66.3</v>
-      </c>
-      <c r="X10" s="3">
-        <v>2304.4</v>
-      </c>
-      <c r="Y10" s="3">
-        <v>21.1</v>
-      </c>
-      <c r="Z10" s="3">
-        <v>-1.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>-161.5</v>
+      </c>
+      <c r="M10">
+        <v>4.8</v>
+      </c>
+      <c r="N10">
+        <v>55</v>
+      </c>
+      <c r="O10">
+        <v>0.8</v>
+      </c>
+      <c r="P10">
+        <v>0.6</v>
+      </c>
+      <c r="Q10">
+        <v>-86.1</v>
+      </c>
+      <c r="R10">
+        <v>2.9</v>
+      </c>
+      <c r="S10">
+        <v>-248.1</v>
+      </c>
+      <c r="T10">
+        <v>24.3</v>
+      </c>
+      <c r="U10">
+        <v>-41.7</v>
+      </c>
+      <c r="V10">
+        <v>2.8</v>
+      </c>
+      <c r="W10">
+        <v>159.1</v>
+      </c>
+      <c r="X10">
+        <v>14.7</v>
+      </c>
+      <c r="Y10">
+        <v>2489.8000000000002</v>
+      </c>
+      <c r="Z10">
+        <v>88.1</v>
+      </c>
+      <c r="AA10">
+        <v>-2.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>33</v>
       </c>
@@ -2479,75 +2552,78 @@
         <v>38</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>30</v>
+        <v>121</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" t="b">
+        <v>73</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K11">
-        <v>-159.4</v>
-      </c>
-      <c r="L11">
+      <c r="L11" s="3">
+        <v>-173.9</v>
+      </c>
+      <c r="M11" s="3">
+        <v>6</v>
+      </c>
+      <c r="N11" s="3">
+        <v>71</v>
+      </c>
+      <c r="O11" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="P11" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>-108.1</v>
+      </c>
+      <c r="R11" s="3">
+        <v>2.9</v>
+      </c>
+      <c r="S11" s="3">
+        <v>-194.3</v>
+      </c>
+      <c r="T11" s="3">
+        <v>13.8</v>
+      </c>
+      <c r="U11" s="3">
+        <v>-43.6</v>
+      </c>
+      <c r="V11" s="3">
         <v>3.4</v>
       </c>
-      <c r="M11">
-        <v>38</v>
-      </c>
-      <c r="N11">
-        <v>0.7</v>
-      </c>
-      <c r="O11">
-        <v>0.4</v>
-      </c>
-      <c r="P11">
-        <v>-93.1</v>
-      </c>
-      <c r="Q11">
-        <v>6.4</v>
-      </c>
-      <c r="R11">
-        <v>-194.1</v>
-      </c>
-      <c r="S11">
-        <v>30</v>
-      </c>
-      <c r="T11">
-        <v>-37.9</v>
-      </c>
-      <c r="U11">
-        <v>7.2</v>
-      </c>
-      <c r="V11">
-        <v>104.7</v>
-      </c>
-      <c r="W11">
-        <v>51.7</v>
-      </c>
-      <c r="X11">
-        <v>2416.6999999999998</v>
-      </c>
-      <c r="Y11">
-        <v>101.2</v>
-      </c>
-      <c r="Z11">
-        <v>-2.4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="W11" s="3">
+        <v>166</v>
+      </c>
+      <c r="X11" s="3">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="Y11" s="3">
+        <v>2677.4</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>64.8</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>-2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>33</v>
       </c>
@@ -2555,75 +2631,78 @@
         <v>38</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>89</v>
+        <v>122</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="3" t="b">
+        <v>46</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K12" s="3">
-        <v>-87.4</v>
-      </c>
       <c r="L12" s="3">
-        <v>3.9</v>
+        <v>-151.30000000000001</v>
       </c>
       <c r="M12" s="3">
-        <v>24</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="N12" s="3">
+        <v>68</v>
+      </c>
+      <c r="O12" s="3">
+        <v>16.2</v>
+      </c>
+      <c r="P12" s="3">
         <v>0.3</v>
       </c>
-      <c r="O12" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="P12" s="3">
-        <v>-48.1</v>
-      </c>
       <c r="Q12" s="3">
-        <v>4.8</v>
+        <v>-86.8</v>
       </c>
       <c r="R12" s="3">
-        <v>-189.2</v>
+        <v>4.5</v>
       </c>
       <c r="S12" s="3">
-        <v>10.4</v>
+        <v>-235.4</v>
       </c>
       <c r="T12" s="3">
-        <v>-23.5</v>
+        <v>9.4</v>
       </c>
       <c r="U12" s="3">
-        <v>2.2999999999999998</v>
+        <v>-29</v>
       </c>
       <c r="V12" s="3">
-        <v>221.4</v>
+        <v>3.7</v>
       </c>
       <c r="W12" s="3">
-        <v>61.7</v>
+        <v>113.6</v>
       </c>
       <c r="X12" s="3">
-        <v>1420.6</v>
+        <v>66.3</v>
       </c>
       <c r="Y12" s="3">
-        <v>10.5</v>
+        <v>2304.4</v>
       </c>
       <c r="Z12" s="3">
-        <v>-2.1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>21.1</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>33</v>
       </c>
@@ -2634,300 +2713,312 @@
         <v>67</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>-159.4</v>
+      </c>
+      <c r="M13">
+        <v>3.4</v>
+      </c>
+      <c r="N13">
+        <v>38</v>
+      </c>
+      <c r="O13">
+        <v>0.7</v>
+      </c>
+      <c r="P13">
+        <v>0.4</v>
+      </c>
+      <c r="Q13">
+        <v>-93.1</v>
+      </c>
+      <c r="R13">
+        <v>6.4</v>
+      </c>
+      <c r="S13">
+        <v>-194.1</v>
+      </c>
+      <c r="T13">
+        <v>30</v>
+      </c>
+      <c r="U13">
+        <v>-37.9</v>
+      </c>
+      <c r="V13">
+        <v>7.2</v>
+      </c>
+      <c r="W13">
+        <v>104.7</v>
+      </c>
+      <c r="X13">
+        <v>51.7</v>
+      </c>
+      <c r="Y13">
+        <v>2416.6999999999998</v>
+      </c>
+      <c r="Z13">
+        <v>101.2</v>
+      </c>
+      <c r="AA13">
+        <v>-2.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L14" s="3">
+        <v>-87.4</v>
+      </c>
+      <c r="M14" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="N14" s="3">
+        <v>24</v>
+      </c>
+      <c r="O14" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="P14" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>-48.1</v>
+      </c>
+      <c r="R14" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="S14" s="3">
+        <v>-189.2</v>
+      </c>
+      <c r="T14" s="3">
+        <v>10.4</v>
+      </c>
+      <c r="U14" s="3">
+        <v>-23.5</v>
+      </c>
+      <c r="V14" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="W14" s="3">
+        <v>221.4</v>
+      </c>
+      <c r="X14" s="3">
+        <v>61.7</v>
+      </c>
+      <c r="Y14" s="3">
+        <v>1420.6</v>
+      </c>
+      <c r="Z14" s="3">
+        <v>10.5</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>-2.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="3" t="b">
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K13" s="3">
+      <c r="L15" s="3">
         <v>-148.9</v>
       </c>
-      <c r="L13" s="3">
+      <c r="M15" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M13" s="3">
+      <c r="N15" s="3">
         <v>52</v>
       </c>
-      <c r="N13" s="3">
+      <c r="O15" s="3">
         <v>0.6</v>
       </c>
-      <c r="O13" s="3">
+      <c r="P15" s="3">
         <v>0.4</v>
       </c>
-      <c r="P13" s="3">
+      <c r="Q15" s="3">
         <v>-94.1</v>
       </c>
-      <c r="Q13" s="3">
+      <c r="R15" s="3">
         <v>3.4</v>
       </c>
-      <c r="R13" s="3">
+      <c r="S15" s="3">
         <v>-191.1</v>
       </c>
-      <c r="S13" s="3">
+      <c r="T15" s="3">
         <v>19.899999999999999</v>
       </c>
-      <c r="T13" s="3">
+      <c r="U15" s="3">
         <v>-30.6</v>
       </c>
-      <c r="U13" s="3">
+      <c r="V15" s="3">
         <v>2.8</v>
       </c>
-      <c r="V13" s="3">
+      <c r="W15" s="3">
         <v>140.4</v>
       </c>
-      <c r="W13" s="3">
+      <c r="X15" s="3">
         <v>44.2</v>
       </c>
-      <c r="X13" s="3">
+      <c r="Y15" s="3">
         <v>2534.5</v>
       </c>
-      <c r="Y13" s="3">
+      <c r="Z15" s="3">
         <v>33.4</v>
       </c>
-      <c r="Z13" s="3">
+      <c r="AA15" s="3">
         <v>-2.1</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" t="s">
-        <v>56</v>
-      </c>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" t="b">
-        <v>1</v>
-      </c>
-      <c r="K14">
-        <v>-156</v>
-      </c>
-      <c r="L14">
-        <v>6.3</v>
-      </c>
-      <c r="M14">
-        <v>50</v>
-      </c>
-      <c r="N14">
-        <v>0.3</v>
-      </c>
-      <c r="O14">
-        <v>0.2</v>
-      </c>
-      <c r="P14">
-        <v>-86.1</v>
-      </c>
-      <c r="Q14">
-        <v>4.8</v>
-      </c>
-      <c r="R14">
-        <v>-354.4</v>
-      </c>
-      <c r="S14">
-        <v>12</v>
-      </c>
-      <c r="T14">
-        <v>-13.8</v>
-      </c>
-      <c r="U14">
-        <v>0.5</v>
-      </c>
-      <c r="V14">
-        <v>147.6</v>
-      </c>
-      <c r="W14">
-        <v>26.9</v>
-      </c>
-      <c r="X14">
-        <v>2479</v>
-      </c>
-      <c r="Y14">
-        <v>50.9</v>
-      </c>
-      <c r="Z14">
-        <v>-2.4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="K15" s="3">
-        <v>-148.1</v>
-      </c>
-      <c r="L15" s="3">
-        <v>2.1</v>
-      </c>
-      <c r="M15" s="3">
-        <v>87</v>
-      </c>
-      <c r="N15" s="3">
-        <v>1</v>
-      </c>
-      <c r="O15" s="3">
-        <v>1</v>
-      </c>
-      <c r="P15" s="3">
-        <v>-89.5</v>
-      </c>
-      <c r="Q15" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="R15" s="3">
-        <v>-254.6</v>
-      </c>
-      <c r="S15" s="3">
-        <v>9.6</v>
-      </c>
-      <c r="T15" s="3">
-        <v>-20.6</v>
-      </c>
-      <c r="U15" s="3">
-        <v>2.9</v>
-      </c>
-      <c r="V15" s="3">
-        <v>129.9</v>
-      </c>
-      <c r="W15" s="3">
-        <v>44.6</v>
-      </c>
-      <c r="X15" s="3">
-        <v>2545.9</v>
-      </c>
-      <c r="Y15" s="3">
-        <v>44.4</v>
-      </c>
-      <c r="Z15" s="3">
-        <v>-2.4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" t="s">
         <v>52</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>75</v>
+        <v>118</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
       </c>
       <c r="F16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="3" t="b">
+      <c r="H16" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" t="b">
         <v>1</v>
       </c>
-      <c r="K16" s="3">
-        <v>-136.1</v>
-      </c>
-      <c r="L16" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="M16" s="3">
-        <v>76</v>
-      </c>
-      <c r="N16" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="O16" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="P16" s="3">
-        <v>-87.6</v>
-      </c>
-      <c r="Q16" s="3">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="R16" s="3">
-        <v>-231.2</v>
-      </c>
-      <c r="S16" s="3">
-        <v>7.3</v>
-      </c>
-      <c r="T16" s="3">
-        <v>-15.4</v>
-      </c>
-      <c r="U16" s="3">
-        <v>1</v>
-      </c>
-      <c r="V16" s="3">
-        <v>131.5</v>
-      </c>
-      <c r="W16" s="3">
-        <v>26.4</v>
-      </c>
-      <c r="X16" s="3">
-        <v>2385.3000000000002</v>
-      </c>
-      <c r="Y16" s="3">
-        <v>104.2</v>
-      </c>
-      <c r="Z16" s="3">
-        <v>-2.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>-156</v>
+      </c>
+      <c r="M16">
+        <v>6.3</v>
+      </c>
+      <c r="N16">
+        <v>50</v>
+      </c>
+      <c r="O16">
+        <v>0.3</v>
+      </c>
+      <c r="P16">
+        <v>0.2</v>
+      </c>
+      <c r="Q16">
+        <v>-86.1</v>
+      </c>
+      <c r="R16">
+        <v>4.8</v>
+      </c>
+      <c r="S16">
+        <v>-354.4</v>
+      </c>
+      <c r="T16">
+        <v>12</v>
+      </c>
+      <c r="U16">
+        <v>-13.8</v>
+      </c>
+      <c r="V16">
+        <v>0.5</v>
+      </c>
+      <c r="W16">
+        <v>147.6</v>
+      </c>
+      <c r="X16">
+        <v>26.9</v>
+      </c>
+      <c r="Y16">
+        <v>2479</v>
+      </c>
+      <c r="Z16">
+        <v>50.9</v>
+      </c>
+      <c r="AA16">
+        <v>-2.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>36</v>
       </c>
@@ -2935,75 +3026,78 @@
         <v>52</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>30</v>
+        <v>121</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" t="b">
+        <v>73</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K17">
-        <v>-99.6</v>
-      </c>
-      <c r="L17">
-        <v>4.7</v>
-      </c>
-      <c r="M17">
-        <v>16</v>
-      </c>
-      <c r="N17">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="O17">
-        <v>0.5</v>
-      </c>
-      <c r="P17">
-        <v>-61.7</v>
-      </c>
-      <c r="Q17">
-        <v>2.5</v>
-      </c>
-      <c r="R17">
-        <v>-171.8</v>
-      </c>
-      <c r="S17">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="T17">
-        <v>-19.5</v>
-      </c>
-      <c r="U17">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="V17">
-        <v>159.4</v>
-      </c>
-      <c r="W17">
-        <v>31.8</v>
-      </c>
-      <c r="X17">
-        <v>1992.6</v>
-      </c>
-      <c r="Y17">
-        <v>123.4</v>
-      </c>
-      <c r="Z17">
-        <v>-1.6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="L17" s="3">
+        <v>-148.1</v>
+      </c>
+      <c r="M17" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="N17" s="3">
+        <v>87</v>
+      </c>
+      <c r="O17" s="3">
+        <v>1</v>
+      </c>
+      <c r="P17" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>-89.5</v>
+      </c>
+      <c r="R17" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="S17" s="3">
+        <v>-254.6</v>
+      </c>
+      <c r="T17" s="3">
+        <v>9.6</v>
+      </c>
+      <c r="U17" s="3">
+        <v>-20.6</v>
+      </c>
+      <c r="V17" s="3">
+        <v>2.9</v>
+      </c>
+      <c r="W17" s="3">
+        <v>129.9</v>
+      </c>
+      <c r="X17" s="3">
+        <v>44.6</v>
+      </c>
+      <c r="Y17" s="3">
+        <v>2545.9</v>
+      </c>
+      <c r="Z17" s="3">
+        <v>44.4</v>
+      </c>
+      <c r="AA17" s="3">
+        <v>-2.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>36</v>
       </c>
@@ -3011,75 +3105,78 @@
         <v>52</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>89</v>
+        <v>122</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="3" t="b">
+        <v>46</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K18" s="3">
-        <v>-43.9</v>
-      </c>
       <c r="L18" s="3">
+        <v>-136.1</v>
+      </c>
+      <c r="M18" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="N18" s="3">
+        <v>76</v>
+      </c>
+      <c r="O18" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="P18" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>-87.6</v>
+      </c>
+      <c r="R18" s="3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="S18" s="3">
+        <v>-231.2</v>
+      </c>
+      <c r="T18" s="3">
+        <v>7.3</v>
+      </c>
+      <c r="U18" s="3">
+        <v>-15.4</v>
+      </c>
+      <c r="V18" s="3">
         <v>1</v>
       </c>
-      <c r="M18" s="3">
-        <v>43</v>
-      </c>
-      <c r="N18" s="3">
-        <v>11.5</v>
-      </c>
-      <c r="O18" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="P18" s="3">
-        <v>-41.1</v>
-      </c>
-      <c r="Q18" s="3">
-        <v>4.7</v>
-      </c>
-      <c r="R18" s="3">
-        <v>-207.9</v>
-      </c>
-      <c r="S18" s="3">
-        <v>33.9</v>
-      </c>
-      <c r="T18" s="3">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="U18" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="V18" s="3">
-        <v>286</v>
-      </c>
       <c r="W18" s="3">
-        <v>42.5</v>
+        <v>131.5</v>
       </c>
       <c r="X18" s="3">
-        <v>1600.2</v>
+        <v>26.4</v>
       </c>
       <c r="Y18" s="3">
-        <v>74.5</v>
+        <v>2385.3000000000002</v>
       </c>
       <c r="Z18" s="3">
-        <v>-1.7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>104.2</v>
+      </c>
+      <c r="AA18" s="3">
+        <v>-2.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>36</v>
       </c>
@@ -3090,300 +3187,312 @@
         <v>67</v>
       </c>
       <c r="D19" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" t="b">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>-99.6</v>
+      </c>
+      <c r="M19">
+        <v>4.7</v>
+      </c>
+      <c r="N19">
+        <v>16</v>
+      </c>
+      <c r="O19">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="P19">
+        <v>0.5</v>
+      </c>
+      <c r="Q19">
+        <v>-61.7</v>
+      </c>
+      <c r="R19">
+        <v>2.5</v>
+      </c>
+      <c r="S19">
+        <v>-171.8</v>
+      </c>
+      <c r="T19">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="U19">
+        <v>-19.5</v>
+      </c>
+      <c r="V19">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="W19">
+        <v>159.4</v>
+      </c>
+      <c r="X19">
+        <v>31.8</v>
+      </c>
+      <c r="Y19">
+        <v>1992.6</v>
+      </c>
+      <c r="Z19">
+        <v>123.4</v>
+      </c>
+      <c r="AA19">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L20" s="3">
+        <v>-43.9</v>
+      </c>
+      <c r="M20" s="3">
+        <v>1</v>
+      </c>
+      <c r="N20" s="3">
+        <v>43</v>
+      </c>
+      <c r="O20" s="3">
+        <v>11.5</v>
+      </c>
+      <c r="P20" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>-41.1</v>
+      </c>
+      <c r="R20" s="3">
+        <v>4.7</v>
+      </c>
+      <c r="S20" s="3">
+        <v>-207.9</v>
+      </c>
+      <c r="T20" s="3">
+        <v>33.9</v>
+      </c>
+      <c r="U20" s="3">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="V20" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="W20" s="3">
+        <v>286</v>
+      </c>
+      <c r="X20" s="3">
+        <v>42.5</v>
+      </c>
+      <c r="Y20" s="3">
+        <v>1600.2</v>
+      </c>
+      <c r="Z20" s="3">
+        <v>74.5</v>
+      </c>
+      <c r="AA20" s="3">
+        <v>-1.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="F21" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="G21" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="H21" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="3" t="b">
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K19" s="3">
+      <c r="L21" s="3">
         <v>-125.4</v>
       </c>
-      <c r="L19" s="3">
+      <c r="M21" s="3">
         <v>12.6</v>
       </c>
-      <c r="M19" s="3">
+      <c r="N21" s="3">
         <v>12</v>
       </c>
-      <c r="N19" s="3">
+      <c r="O21" s="3">
         <v>0.8</v>
       </c>
-      <c r="O19" s="3">
+      <c r="P21" s="3">
         <v>0.6</v>
       </c>
-      <c r="P19" s="3">
+      <c r="Q21" s="3">
         <v>-81.900000000000006</v>
       </c>
-      <c r="Q19" s="3">
+      <c r="R21" s="3">
         <v>8.6999999999999993</v>
       </c>
-      <c r="R19" s="3">
+      <c r="S21" s="3">
         <v>-223.5</v>
       </c>
-      <c r="S19" s="3">
+      <c r="T21" s="3">
         <v>21.4</v>
       </c>
-      <c r="T19" s="3">
+      <c r="U21" s="3">
         <v>-8</v>
       </c>
-      <c r="U19" s="3">
+      <c r="V21" s="3">
         <v>3.1</v>
       </c>
-      <c r="V19" s="3">
+      <c r="W21" s="3">
         <v>92.5</v>
       </c>
-      <c r="W19" s="3">
+      <c r="X21" s="3">
         <v>50.5</v>
       </c>
-      <c r="X19" s="3">
+      <c r="Y21" s="3">
         <v>2301.1</v>
       </c>
-      <c r="Y19" s="3">
+      <c r="Z21" s="3">
         <v>54.4</v>
       </c>
-      <c r="Z19" s="3">
+      <c r="AA21" s="3">
         <v>-1.6</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="K20">
-        <v>-144.4</v>
-      </c>
-      <c r="L20">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="M20">
-        <v>73</v>
-      </c>
-      <c r="N20">
-        <v>1.8</v>
-      </c>
-      <c r="O20">
-        <v>1.4</v>
-      </c>
-      <c r="P20">
-        <v>-85</v>
-      </c>
-      <c r="Q20">
-        <v>5.6</v>
-      </c>
-      <c r="R20">
-        <v>-280.89999999999998</v>
-      </c>
-      <c r="S20">
-        <v>23.9</v>
-      </c>
-      <c r="T20">
-        <v>-18.899999999999999</v>
-      </c>
-      <c r="U20">
-        <v>3.2</v>
-      </c>
-      <c r="V20">
-        <v>154.1</v>
-      </c>
-      <c r="W20">
-        <v>39.700000000000003</v>
-      </c>
-      <c r="X20">
-        <v>2417.8000000000002</v>
-      </c>
-      <c r="Y20">
-        <v>163.9</v>
-      </c>
-      <c r="Z20">
-        <v>-2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K21" s="3">
-        <v>-139.6</v>
-      </c>
-      <c r="L21" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="M21" s="3">
-        <v>50</v>
-      </c>
-      <c r="N21" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="O21" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="P21" s="3">
-        <v>-78.599999999999994</v>
-      </c>
-      <c r="Q21" s="3">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="R21" s="3">
-        <v>-256.10000000000002</v>
-      </c>
-      <c r="S21" s="3">
-        <v>61.8</v>
-      </c>
-      <c r="T21" s="3">
-        <v>-31.9</v>
-      </c>
-      <c r="U21" s="3">
-        <v>6.3</v>
-      </c>
-      <c r="V21" s="3">
-        <v>221.4</v>
-      </c>
-      <c r="W21" s="3">
-        <v>43.9</v>
-      </c>
-      <c r="X21" s="3">
-        <v>2407.5</v>
-      </c>
-      <c r="Y21" s="3">
-        <v>137.6</v>
-      </c>
-      <c r="Z21" s="3">
-        <v>-1.8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" t="s">
         <v>55</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>75</v>
+        <v>118</v>
+      </c>
+      <c r="E22" t="s">
+        <v>54</v>
       </c>
       <c r="F22" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="3" t="b">
+      <c r="H22" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K22" s="3">
-        <v>-174.1</v>
-      </c>
-      <c r="L22" s="3">
-        <v>7.2</v>
-      </c>
-      <c r="M22" s="3">
-        <v>42</v>
-      </c>
-      <c r="N22" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="O22" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="P22" s="3">
-        <v>-95</v>
-      </c>
-      <c r="Q22" s="3">
+      <c r="L22">
+        <v>-144.4</v>
+      </c>
+      <c r="M22">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N22">
+        <v>73</v>
+      </c>
+      <c r="O22">
+        <v>1.8</v>
+      </c>
+      <c r="P22">
+        <v>1.4</v>
+      </c>
+      <c r="Q22">
+        <v>-85</v>
+      </c>
+      <c r="R22">
+        <v>5.6</v>
+      </c>
+      <c r="S22">
+        <v>-280.89999999999998</v>
+      </c>
+      <c r="T22">
+        <v>23.9</v>
+      </c>
+      <c r="U22">
+        <v>-18.899999999999999</v>
+      </c>
+      <c r="V22">
         <v>3.2</v>
       </c>
-      <c r="R22" s="3">
-        <v>-379.8</v>
-      </c>
-      <c r="S22" s="3">
-        <v>61</v>
-      </c>
-      <c r="T22" s="3">
-        <v>-20.8</v>
-      </c>
-      <c r="U22" s="3">
-        <v>6.6</v>
-      </c>
-      <c r="V22" s="3">
-        <v>176.2</v>
-      </c>
-      <c r="W22" s="3">
-        <v>22</v>
-      </c>
-      <c r="X22" s="3">
-        <v>2766.9</v>
-      </c>
-      <c r="Y22" s="3">
-        <v>89.3</v>
-      </c>
-      <c r="Z22" s="3">
-        <v>-1.8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="W22">
+        <v>154.1</v>
+      </c>
+      <c r="X22">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="Y22">
+        <v>2417.8000000000002</v>
+      </c>
+      <c r="Z22">
+        <v>163.9</v>
+      </c>
+      <c r="AA22">
+        <v>-2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>32</v>
       </c>
@@ -3391,75 +3500,78 @@
         <v>55</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>30</v>
+        <v>121</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" t="b">
+        <v>73</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="K23">
-        <v>-126.8</v>
-      </c>
-      <c r="L23">
-        <v>1.2</v>
-      </c>
-      <c r="M23">
-        <v>26</v>
-      </c>
-      <c r="N23">
-        <v>13.6</v>
-      </c>
-      <c r="O23">
-        <v>0.8</v>
-      </c>
-      <c r="P23">
-        <v>-71.8</v>
-      </c>
-      <c r="Q23">
-        <v>4.2</v>
-      </c>
-      <c r="R23">
-        <v>-268.89999999999998</v>
-      </c>
-      <c r="S23">
-        <v>19.3</v>
-      </c>
-      <c r="T23">
-        <v>-17.100000000000001</v>
-      </c>
-      <c r="U23">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="V23">
-        <v>158.80000000000001</v>
-      </c>
-      <c r="W23">
-        <v>44.7</v>
-      </c>
-      <c r="X23">
-        <v>2299.6</v>
-      </c>
-      <c r="Y23">
-        <v>139.69999999999999</v>
-      </c>
-      <c r="Z23">
-        <v>-2.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="L23" s="3">
+        <v>-139.6</v>
+      </c>
+      <c r="M23" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="N23" s="3">
+        <v>50</v>
+      </c>
+      <c r="O23" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="P23" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>-78.599999999999994</v>
+      </c>
+      <c r="R23" s="3">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="S23" s="3">
+        <v>-256.10000000000002</v>
+      </c>
+      <c r="T23" s="3">
+        <v>61.8</v>
+      </c>
+      <c r="U23" s="3">
+        <v>-31.9</v>
+      </c>
+      <c r="V23" s="3">
+        <v>6.3</v>
+      </c>
+      <c r="W23" s="3">
+        <v>221.4</v>
+      </c>
+      <c r="X23" s="3">
+        <v>43.9</v>
+      </c>
+      <c r="Y23" s="3">
+        <v>2407.5</v>
+      </c>
+      <c r="Z23" s="3">
+        <v>137.6</v>
+      </c>
+      <c r="AA23" s="3">
+        <v>-1.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>32</v>
       </c>
@@ -3467,75 +3579,78 @@
         <v>55</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>89</v>
+        <v>122</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="3" t="b">
+        <v>46</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K24" s="3">
-        <v>-78.400000000000006</v>
-      </c>
       <c r="L24" s="3">
-        <v>2.5</v>
+        <v>-174.1</v>
       </c>
       <c r="M24" s="3">
-        <v>36</v>
+        <v>7.2</v>
       </c>
       <c r="N24" s="3">
-        <v>0.2</v>
+        <v>42</v>
       </c>
       <c r="O24" s="3">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="P24" s="3">
-        <v>-44.2</v>
+        <v>0.4</v>
       </c>
       <c r="Q24" s="3">
-        <v>3</v>
+        <v>-95</v>
       </c>
       <c r="R24" s="3">
-        <v>-324.5</v>
+        <v>3.2</v>
       </c>
       <c r="S24" s="3">
-        <v>15</v>
+        <v>-379.8</v>
       </c>
       <c r="T24" s="3">
-        <v>-3.2</v>
+        <v>61</v>
       </c>
       <c r="U24" s="3">
-        <v>0.3</v>
+        <v>-20.8</v>
       </c>
       <c r="V24" s="3">
-        <v>338.6</v>
+        <v>6.6</v>
       </c>
       <c r="W24" s="3">
-        <v>21.2</v>
+        <v>176.2</v>
       </c>
       <c r="X24" s="3">
-        <v>1555.1</v>
+        <v>22</v>
       </c>
       <c r="Y24" s="3">
-        <v>16.399999999999999</v>
+        <v>2766.9</v>
       </c>
       <c r="Z24" s="3">
-        <v>-1.9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>89.3</v>
+      </c>
+      <c r="AA24" s="3">
+        <v>-1.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>32</v>
       </c>
@@ -3546,76 +3661,237 @@
         <v>67</v>
       </c>
       <c r="D25" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" t="b">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>-126.8</v>
+      </c>
+      <c r="M25">
+        <v>1.2</v>
+      </c>
+      <c r="N25">
+        <v>26</v>
+      </c>
+      <c r="O25">
+        <v>13.6</v>
+      </c>
+      <c r="P25">
+        <v>0.8</v>
+      </c>
+      <c r="Q25">
+        <v>-71.8</v>
+      </c>
+      <c r="R25">
+        <v>4.2</v>
+      </c>
+      <c r="S25">
+        <v>-268.89999999999998</v>
+      </c>
+      <c r="T25">
+        <v>19.3</v>
+      </c>
+      <c r="U25">
+        <v>-17.100000000000001</v>
+      </c>
+      <c r="V25">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="W25">
+        <v>158.80000000000001</v>
+      </c>
+      <c r="X25">
+        <v>44.7</v>
+      </c>
+      <c r="Y25">
+        <v>2299.6</v>
+      </c>
+      <c r="Z25">
+        <v>139.69999999999999</v>
+      </c>
+      <c r="AA25">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L26" s="3">
+        <v>-78.400000000000006</v>
+      </c>
+      <c r="M26" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="N26" s="3">
+        <v>36</v>
+      </c>
+      <c r="O26" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="P26" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>-44.2</v>
+      </c>
+      <c r="R26" s="3">
+        <v>3</v>
+      </c>
+      <c r="S26" s="3">
+        <v>-324.5</v>
+      </c>
+      <c r="T26" s="3">
+        <v>15</v>
+      </c>
+      <c r="U26" s="3">
+        <v>-3.2</v>
+      </c>
+      <c r="V26" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="W26" s="3">
+        <v>338.6</v>
+      </c>
+      <c r="X26" s="3">
+        <v>21.2</v>
+      </c>
+      <c r="Y26" s="3">
+        <v>1555.1</v>
+      </c>
+      <c r="Z26" s="3">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="AA26" s="3">
+        <v>-1.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="F27" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="G27" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="H27" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="3" t="b">
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K25" s="3">
+      <c r="L27" s="3">
         <v>-120</v>
       </c>
-      <c r="L25" s="3">
+      <c r="M27" s="3">
         <v>4.2</v>
       </c>
-      <c r="M25" s="3">
+      <c r="N27" s="3">
         <v>8</v>
       </c>
-      <c r="N25" s="3">
+      <c r="O27" s="3">
         <v>16.5</v>
       </c>
-      <c r="O25" s="3">
+      <c r="P27" s="3">
         <v>0.2</v>
       </c>
-      <c r="P25" s="3">
+      <c r="Q27" s="3">
         <v>-67</v>
       </c>
-      <c r="Q25" s="3">
+      <c r="R27" s="3">
         <v>5.6</v>
       </c>
-      <c r="R25" s="3">
+      <c r="S27" s="3">
         <v>-271</v>
       </c>
-      <c r="S25" s="3">
+      <c r="T27" s="3">
         <v>14.7</v>
       </c>
-      <c r="T25" s="3">
+      <c r="U27" s="3">
         <v>-17.2</v>
       </c>
-      <c r="U25" s="3">
+      <c r="V27" s="3">
         <v>5.4</v>
       </c>
-      <c r="V25" s="3">
+      <c r="W27" s="3">
         <v>183.8</v>
       </c>
-      <c r="W25" s="3">
+      <c r="X27" s="3">
         <v>62.5</v>
       </c>
-      <c r="X25" s="3">
+      <c r="Y27" s="3">
         <v>1979.8</v>
       </c>
-      <c r="Y25" s="3">
+      <c r="Z27" s="3">
         <v>99.6</v>
       </c>
-      <c r="Z25" s="3">
+      <c r="AA27" s="3">
         <v>-2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z5" xr:uid="{30842AB1-A644-42C7-A90C-F34DF0E50414}"/>
+  <autoFilter ref="A1:AA5" xr:uid="{30842AB1-A644-42C7-A90C-F34DF0E50414}"/>
   <mergeCells count="2">
-    <mergeCell ref="H2:H25"/>
-    <mergeCell ref="I2:I25"/>
+    <mergeCell ref="I2:I27"/>
+    <mergeCell ref="J2:J27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3627,7 +3903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EB7B74B-0B0F-4759-A970-25E74CC533ED}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -3642,7 +3918,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>49</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -3650,7 +3926,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>103</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -3664,72 +3940,72 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <v>-198.6</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>-161.19166666666663</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>-136.1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <v>-163.30000000000001</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>-137.27500000000001</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>-99.6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <v>-87.4</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="10">
         <v>-70.325000000000003</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <v>-43.9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="10">
         <v>-148.9</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <v>-128.19999999999999</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <v>-118.5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <v>-198.6</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <v>-136.56250000000003</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <v>-43.9</v>
       </c>
     </row>

</xml_diff>